<commit_message>
Added new words to translations
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="1901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="1904">
   <si>
     <t>Key</t>
   </si>
@@ -5726,6 +5726,15 @@
   </si>
   <si>
     <t>newVisit.PLACEHOLDER-educationGoals.3</t>
+  </si>
+  <si>
+    <t>referral.pending</t>
+  </si>
+  <si>
+    <t>Pending Referrals</t>
+  </si>
+  <si>
+    <t>&amp;Pending Referrals</t>
   </si>
 </sst>
 </file>
@@ -14973,7 +14982,17 @@
         <v>&amp;No goals</v>
       </c>
     </row>
-    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1">
+      <c r="A686" s="26" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B686" s="12" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C686" s="12" t="s">
+        <v>1903</v>
+      </c>
+    </row>
     <row r="687" ht="15.75" customHeight="1"/>
     <row r="688" ht="15.75" customHeight="1"/>
     <row r="689" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added filter by referral types
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="1904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="1907">
   <si>
     <t>Key</t>
   </si>
@@ -5735,6 +5735,15 @@
   </si>
   <si>
     <t>&amp;Pending Referrals</t>
+  </si>
+  <si>
+    <t>referral.filterByType</t>
+  </si>
+  <si>
+    <t>Filter by Referral Types</t>
+  </si>
+  <si>
+    <t>&amp;Filter by Referral Types</t>
   </si>
 </sst>
 </file>
@@ -5780,7 +5789,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5797,6 +5806,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEA9999"/>
         <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE06666"/>
+        <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
     <fill>
@@ -5818,7 +5833,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5860,7 +5875,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5869,25 +5885,25 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9864,7 +9880,7 @@
       <c r="E287" s="4"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="7" t="s">
+      <c r="A288" s="19" t="s">
         <v>836</v>
       </c>
       <c r="B288" s="8" t="s">
@@ -12854,10 +12870,10 @@
       <c r="E517" s="4"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="A518" s="19" t="s">
+      <c r="A518" s="20" t="s">
         <v>1451</v>
       </c>
-      <c r="B518" s="20" t="s">
+      <c r="B518" s="21" t="s">
         <v>1452</v>
       </c>
       <c r="C518" s="12" t="s">
@@ -12867,10 +12883,10 @@
       <c r="E518" s="4"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="A519" s="19" t="s">
+      <c r="A519" s="20" t="s">
         <v>1454</v>
       </c>
-      <c r="B519" s="20" t="s">
+      <c r="B519" s="21" t="s">
         <v>1455</v>
       </c>
       <c r="C519" s="12" t="s">
@@ -12880,1279 +12896,1279 @@
       <c r="E519" s="4"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="A520" s="19" t="s">
+      <c r="A520" s="20" t="s">
         <v>1457</v>
       </c>
-      <c r="B520" s="20" t="s">
+      <c r="B520" s="21" t="s">
         <v>1458</v>
       </c>
-      <c r="C520" s="20" t="s">
+      <c r="C520" s="21" t="s">
         <v>1459</v>
       </c>
-      <c r="D520" s="20"/>
+      <c r="D520" s="21"/>
       <c r="E520" s="4"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="A521" s="19" t="s">
+      <c r="A521" s="20" t="s">
         <v>1460</v>
       </c>
-      <c r="B521" s="20" t="s">
+      <c r="B521" s="21" t="s">
         <v>1461</v>
       </c>
-      <c r="C521" s="20" t="s">
+      <c r="C521" s="21" t="s">
         <v>1462</v>
       </c>
-      <c r="D521" s="20"/>
+      <c r="D521" s="21"/>
       <c r="E521" s="4"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="A522" s="19" t="s">
+      <c r="A522" s="20" t="s">
         <v>1463</v>
       </c>
-      <c r="B522" s="20" t="s">
+      <c r="B522" s="21" t="s">
         <v>1464</v>
       </c>
-      <c r="C522" s="20" t="s">
+      <c r="C522" s="21" t="s">
         <v>1465</v>
       </c>
-      <c r="D522" s="20"/>
+      <c r="D522" s="21"/>
       <c r="E522" s="4"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="A523" s="19" t="s">
+      <c r="A523" s="20" t="s">
         <v>1466</v>
       </c>
-      <c r="B523" s="20" t="s">
+      <c r="B523" s="21" t="s">
         <v>1467</v>
       </c>
-      <c r="C523" s="20" t="s">
+      <c r="C523" s="21" t="s">
         <v>1468</v>
       </c>
-      <c r="D523" s="20"/>
+      <c r="D523" s="21"/>
       <c r="E523" s="4"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="A524" s="19" t="s">
+      <c r="A524" s="20" t="s">
         <v>1469</v>
       </c>
-      <c r="B524" s="20" t="s">
+      <c r="B524" s="21" t="s">
         <v>1470</v>
       </c>
-      <c r="C524" s="20" t="s">
+      <c r="C524" s="21" t="s">
         <v>1471</v>
       </c>
-      <c r="D524" s="20"/>
+      <c r="D524" s="21"/>
       <c r="E524" s="4"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="A525" s="19" t="s">
+      <c r="A525" s="20" t="s">
         <v>1472</v>
       </c>
-      <c r="B525" s="20" t="s">
+      <c r="B525" s="21" t="s">
         <v>1473</v>
       </c>
-      <c r="C525" s="20" t="s">
+      <c r="C525" s="21" t="s">
         <v>1474</v>
       </c>
-      <c r="D525" s="20"/>
+      <c r="D525" s="21"/>
       <c r="E525" s="4"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="A526" s="19" t="s">
+      <c r="A526" s="20" t="s">
         <v>1475</v>
       </c>
-      <c r="B526" s="20" t="s">
+      <c r="B526" s="21" t="s">
         <v>1476</v>
       </c>
-      <c r="C526" s="20" t="s">
+      <c r="C526" s="21" t="s">
         <v>1477</v>
       </c>
-      <c r="D526" s="20"/>
+      <c r="D526" s="21"/>
       <c r="E526" s="4"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="A527" s="19" t="s">
+      <c r="A527" s="20" t="s">
         <v>1478</v>
       </c>
-      <c r="B527" s="20" t="s">
+      <c r="B527" s="21" t="s">
         <v>1479</v>
       </c>
-      <c r="C527" s="20" t="s">
+      <c r="C527" s="21" t="s">
         <v>1480</v>
       </c>
-      <c r="D527" s="20"/>
+      <c r="D527" s="21"/>
       <c r="E527" s="4"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="A528" s="19" t="s">
+      <c r="A528" s="20" t="s">
         <v>1481</v>
       </c>
-      <c r="B528" s="20" t="s">
+      <c r="B528" s="21" t="s">
         <v>1482</v>
       </c>
-      <c r="C528" s="20" t="s">
+      <c r="C528" s="21" t="s">
         <v>1483</v>
       </c>
-      <c r="D528" s="20"/>
+      <c r="D528" s="21"/>
       <c r="E528" s="4"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="A529" s="19" t="s">
+      <c r="A529" s="20" t="s">
         <v>1484</v>
       </c>
-      <c r="B529" s="20" t="s">
+      <c r="B529" s="21" t="s">
         <v>1485</v>
       </c>
-      <c r="C529" s="20" t="s">
+      <c r="C529" s="21" t="s">
         <v>1486</v>
       </c>
-      <c r="D529" s="20"/>
+      <c r="D529" s="21"/>
       <c r="E529" s="4"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="A530" s="19" t="s">
+      <c r="A530" s="20" t="s">
         <v>1487</v>
       </c>
-      <c r="B530" s="20" t="s">
+      <c r="B530" s="21" t="s">
         <v>1488</v>
       </c>
-      <c r="C530" s="20" t="s">
+      <c r="C530" s="21" t="s">
         <v>1489</v>
       </c>
-      <c r="D530" s="20"/>
+      <c r="D530" s="21"/>
       <c r="E530" s="4"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="A531" s="19" t="s">
+      <c r="A531" s="20" t="s">
         <v>1490</v>
       </c>
-      <c r="B531" s="20" t="s">
+      <c r="B531" s="21" t="s">
         <v>1491</v>
       </c>
-      <c r="C531" s="20" t="s">
+      <c r="C531" s="21" t="s">
         <v>1492</v>
       </c>
-      <c r="D531" s="20"/>
+      <c r="D531" s="21"/>
       <c r="E531" s="4"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="A532" s="19" t="s">
+      <c r="A532" s="20" t="s">
         <v>1493</v>
       </c>
-      <c r="B532" s="20" t="s">
+      <c r="B532" s="21" t="s">
         <v>1494</v>
       </c>
-      <c r="C532" s="20" t="s">
+      <c r="C532" s="21" t="s">
         <v>1495</v>
       </c>
-      <c r="D532" s="20"/>
+      <c r="D532" s="21"/>
       <c r="E532" s="4"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="A533" s="19" t="s">
+      <c r="A533" s="20" t="s">
         <v>1496</v>
       </c>
-      <c r="B533" s="20" t="s">
+      <c r="B533" s="21" t="s">
         <v>1497</v>
       </c>
-      <c r="C533" s="20" t="s">
+      <c r="C533" s="21" t="s">
         <v>1498</v>
       </c>
-      <c r="D533" s="20"/>
+      <c r="D533" s="21"/>
       <c r="E533" s="4"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="A534" s="19" t="s">
+      <c r="A534" s="20" t="s">
         <v>1499</v>
       </c>
-      <c r="B534" s="20" t="s">
+      <c r="B534" s="21" t="s">
         <v>1500</v>
       </c>
-      <c r="C534" s="20" t="s">
+      <c r="C534" s="21" t="s">
         <v>1501</v>
       </c>
-      <c r="D534" s="20"/>
+      <c r="D534" s="21"/>
       <c r="E534" s="4"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="A535" s="19" t="s">
+      <c r="A535" s="20" t="s">
         <v>1502</v>
       </c>
-      <c r="B535" s="20" t="s">
+      <c r="B535" s="21" t="s">
         <v>1503</v>
       </c>
-      <c r="C535" s="20" t="s">
+      <c r="C535" s="21" t="s">
         <v>1504</v>
       </c>
-      <c r="D535" s="20"/>
+      <c r="D535" s="21"/>
       <c r="E535" s="4"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="A536" s="19" t="s">
+      <c r="A536" s="20" t="s">
         <v>1505</v>
       </c>
-      <c r="B536" s="20" t="s">
+      <c r="B536" s="21" t="s">
         <v>1506</v>
       </c>
-      <c r="C536" s="20" t="s">
+      <c r="C536" s="21" t="s">
         <v>1507</v>
       </c>
-      <c r="D536" s="20"/>
+      <c r="D536" s="21"/>
       <c r="E536" s="4"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="A537" s="19" t="s">
+      <c r="A537" s="20" t="s">
         <v>1508</v>
       </c>
-      <c r="B537" s="20" t="s">
+      <c r="B537" s="21" t="s">
         <v>1509</v>
       </c>
-      <c r="C537" s="20" t="s">
+      <c r="C537" s="21" t="s">
         <v>1510</v>
       </c>
-      <c r="D537" s="20"/>
+      <c r="D537" s="21"/>
       <c r="E537" s="4"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="A538" s="19" t="s">
+      <c r="A538" s="20" t="s">
         <v>1511</v>
       </c>
-      <c r="B538" s="20" t="s">
+      <c r="B538" s="21" t="s">
         <v>1512</v>
       </c>
-      <c r="C538" s="20" t="s">
+      <c r="C538" s="21" t="s">
         <v>1513</v>
       </c>
-      <c r="D538" s="20"/>
+      <c r="D538" s="21"/>
       <c r="E538" s="4"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="A539" s="19" t="s">
+      <c r="A539" s="20" t="s">
         <v>1514</v>
       </c>
-      <c r="B539" s="20" t="s">
+      <c r="B539" s="21" t="s">
         <v>1515</v>
       </c>
-      <c r="C539" s="20" t="s">
+      <c r="C539" s="21" t="s">
         <v>1516</v>
       </c>
-      <c r="D539" s="20"/>
+      <c r="D539" s="21"/>
       <c r="E539" s="4"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="A540" s="19" t="s">
+      <c r="A540" s="20" t="s">
         <v>1517</v>
       </c>
-      <c r="B540" s="20" t="s">
+      <c r="B540" s="21" t="s">
         <v>1518</v>
       </c>
-      <c r="C540" s="20" t="s">
+      <c r="C540" s="21" t="s">
         <v>1519</v>
       </c>
-      <c r="D540" s="20"/>
+      <c r="D540" s="21"/>
       <c r="E540" s="4"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="A541" s="19" t="s">
+      <c r="A541" s="20" t="s">
         <v>1520</v>
       </c>
-      <c r="B541" s="20" t="s">
+      <c r="B541" s="21" t="s">
         <v>1521</v>
       </c>
-      <c r="C541" s="20" t="s">
+      <c r="C541" s="21" t="s">
         <v>1522</v>
       </c>
-      <c r="D541" s="20"/>
+      <c r="D541" s="21"/>
       <c r="E541" s="4"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="A542" s="19" t="s">
+      <c r="A542" s="20" t="s">
         <v>1523</v>
       </c>
-      <c r="B542" s="20" t="s">
+      <c r="B542" s="21" t="s">
         <v>1524</v>
       </c>
-      <c r="C542" s="20" t="s">
+      <c r="C542" s="21" t="s">
         <v>1525</v>
       </c>
-      <c r="D542" s="20"/>
+      <c r="D542" s="21"/>
       <c r="E542" s="4"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="A543" s="19" t="s">
+      <c r="A543" s="20" t="s">
         <v>1526</v>
       </c>
-      <c r="B543" s="20" t="s">
+      <c r="B543" s="21" t="s">
         <v>1527</v>
       </c>
-      <c r="C543" s="20" t="s">
+      <c r="C543" s="21" t="s">
         <v>1528</v>
       </c>
-      <c r="D543" s="20"/>
+      <c r="D543" s="21"/>
       <c r="E543" s="4"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="A544" s="19" t="s">
+      <c r="A544" s="20" t="s">
         <v>1529</v>
       </c>
-      <c r="B544" s="20" t="s">
+      <c r="B544" s="21" t="s">
         <v>1530</v>
       </c>
-      <c r="C544" s="20" t="s">
+      <c r="C544" s="21" t="s">
         <v>1531</v>
       </c>
-      <c r="D544" s="20"/>
+      <c r="D544" s="21"/>
       <c r="E544" s="4"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="A545" s="19" t="s">
+      <c r="A545" s="20" t="s">
         <v>1532</v>
       </c>
-      <c r="B545" s="20" t="s">
+      <c r="B545" s="21" t="s">
         <v>1533</v>
       </c>
-      <c r="C545" s="20" t="s">
+      <c r="C545" s="21" t="s">
         <v>1534</v>
       </c>
-      <c r="D545" s="20"/>
+      <c r="D545" s="21"/>
       <c r="E545" s="4"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="A546" s="19" t="s">
+      <c r="A546" s="20" t="s">
         <v>1535</v>
       </c>
-      <c r="B546" s="20" t="s">
+      <c r="B546" s="21" t="s">
         <v>1536</v>
       </c>
-      <c r="C546" s="20" t="s">
+      <c r="C546" s="21" t="s">
         <v>1537</v>
       </c>
-      <c r="D546" s="20"/>
+      <c r="D546" s="21"/>
       <c r="E546" s="4"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="A547" s="19" t="s">
+      <c r="A547" s="20" t="s">
         <v>1538</v>
       </c>
-      <c r="B547" s="20" t="s">
+      <c r="B547" s="21" t="s">
         <v>1539</v>
       </c>
-      <c r="C547" s="20" t="s">
+      <c r="C547" s="21" t="s">
         <v>1540</v>
       </c>
-      <c r="D547" s="20"/>
+      <c r="D547" s="21"/>
       <c r="E547" s="4"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="A548" s="19" t="s">
+      <c r="A548" s="20" t="s">
         <v>1541</v>
       </c>
-      <c r="B548" s="20" t="s">
+      <c r="B548" s="21" t="s">
         <v>1542</v>
       </c>
-      <c r="C548" s="20" t="s">
+      <c r="C548" s="21" t="s">
         <v>1543</v>
       </c>
-      <c r="D548" s="20"/>
+      <c r="D548" s="21"/>
       <c r="E548" s="4"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="A549" s="19" t="s">
+      <c r="A549" s="20" t="s">
         <v>1544</v>
       </c>
-      <c r="B549" s="20" t="s">
+      <c r="B549" s="21" t="s">
         <v>1545</v>
       </c>
-      <c r="C549" s="20" t="s">
+      <c r="C549" s="21" t="s">
         <v>1546</v>
       </c>
-      <c r="D549" s="20"/>
+      <c r="D549" s="21"/>
       <c r="E549" s="4"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="A550" s="19" t="s">
+      <c r="A550" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="B550" s="20" t="s">
+      <c r="B550" s="21" t="s">
         <v>1548</v>
       </c>
-      <c r="C550" s="20" t="s">
+      <c r="C550" s="21" t="s">
         <v>1549</v>
       </c>
-      <c r="D550" s="20"/>
+      <c r="D550" s="21"/>
       <c r="E550" s="4"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="A551" s="19" t="s">
+      <c r="A551" s="20" t="s">
         <v>1550</v>
       </c>
-      <c r="B551" s="20" t="s">
+      <c r="B551" s="21" t="s">
         <v>1551</v>
       </c>
-      <c r="C551" s="20" t="s">
+      <c r="C551" s="21" t="s">
         <v>1552</v>
       </c>
-      <c r="D551" s="20"/>
+      <c r="D551" s="21"/>
       <c r="E551" s="4"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="A552" s="19" t="s">
+      <c r="A552" s="20" t="s">
         <v>1553</v>
       </c>
-      <c r="B552" s="20" t="s">
+      <c r="B552" s="21" t="s">
         <v>1554</v>
       </c>
-      <c r="C552" s="20" t="s">
+      <c r="C552" s="21" t="s">
         <v>1555</v>
       </c>
-      <c r="D552" s="20"/>
+      <c r="D552" s="21"/>
       <c r="E552" s="4"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="A553" s="19" t="s">
+      <c r="A553" s="20" t="s">
         <v>1556</v>
       </c>
-      <c r="B553" s="21" t="s">
+      <c r="B553" s="22" t="s">
         <v>1557</v>
       </c>
-      <c r="C553" s="21" t="s">
+      <c r="C553" s="22" t="s">
         <v>1558</v>
       </c>
-      <c r="D553" s="20"/>
+      <c r="D553" s="21"/>
       <c r="E553" s="4"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="A554" s="22" t="s">
+      <c r="A554" s="23" t="s">
         <v>1559</v>
       </c>
-      <c r="B554" s="23" t="s">
+      <c r="B554" s="24" t="s">
         <v>1560</v>
       </c>
-      <c r="C554" s="23" t="s">
+      <c r="C554" s="24" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="A555" s="19" t="s">
+      <c r="A555" s="20" t="s">
         <v>1562</v>
       </c>
-      <c r="B555" s="20" t="s">
+      <c r="B555" s="21" t="s">
         <v>1563</v>
       </c>
-      <c r="C555" s="20" t="s">
+      <c r="C555" s="21" t="s">
         <v>1564</v>
       </c>
-      <c r="D555" s="20"/>
+      <c r="D555" s="21"/>
       <c r="E555" s="4"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="A556" s="19" t="s">
+      <c r="A556" s="20" t="s">
         <v>1565</v>
       </c>
-      <c r="B556" s="20" t="s">
+      <c r="B556" s="21" t="s">
         <v>1566</v>
       </c>
-      <c r="C556" s="20" t="s">
+      <c r="C556" s="21" t="s">
         <v>1567</v>
       </c>
-      <c r="D556" s="20"/>
+      <c r="D556" s="21"/>
       <c r="E556" s="4"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="A557" s="19" t="s">
+      <c r="A557" s="20" t="s">
         <v>1568</v>
       </c>
-      <c r="B557" s="20" t="s">
+      <c r="B557" s="21" t="s">
         <v>1569</v>
       </c>
-      <c r="C557" s="20" t="s">
+      <c r="C557" s="21" t="s">
         <v>1570</v>
       </c>
-      <c r="D557" s="20"/>
+      <c r="D557" s="21"/>
       <c r="E557" s="4"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="A558" s="19" t="s">
+      <c r="A558" s="20" t="s">
         <v>1571</v>
       </c>
-      <c r="B558" s="20" t="s">
+      <c r="B558" s="21" t="s">
         <v>1572</v>
       </c>
-      <c r="C558" s="20" t="s">
+      <c r="C558" s="21" t="s">
         <v>1573</v>
       </c>
-      <c r="D558" s="20"/>
+      <c r="D558" s="21"/>
       <c r="E558" s="4"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="A559" s="19" t="s">
+      <c r="A559" s="20" t="s">
         <v>1574</v>
       </c>
-      <c r="B559" s="20" t="s">
+      <c r="B559" s="21" t="s">
         <v>1575</v>
       </c>
-      <c r="C559" s="20" t="s">
+      <c r="C559" s="21" t="s">
         <v>1576</v>
       </c>
-      <c r="D559" s="20"/>
+      <c r="D559" s="21"/>
       <c r="E559" s="4"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="A560" s="19" t="s">
+      <c r="A560" s="20" t="s">
         <v>1577</v>
       </c>
-      <c r="B560" s="20" t="s">
+      <c r="B560" s="21" t="s">
         <v>1578</v>
       </c>
-      <c r="C560" s="20" t="s">
+      <c r="C560" s="21" t="s">
         <v>1579</v>
       </c>
-      <c r="D560" s="20"/>
+      <c r="D560" s="21"/>
       <c r="E560" s="4"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="A561" s="19" t="s">
+      <c r="A561" s="20" t="s">
         <v>1580</v>
       </c>
-      <c r="B561" s="20" t="s">
+      <c r="B561" s="21" t="s">
         <v>1581</v>
       </c>
-      <c r="C561" s="20" t="s">
+      <c r="C561" s="21" t="s">
         <v>1582</v>
       </c>
-      <c r="D561" s="20"/>
+      <c r="D561" s="21"/>
       <c r="E561" s="4"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="A562" s="19" t="s">
+      <c r="A562" s="20" t="s">
         <v>1583</v>
       </c>
-      <c r="B562" s="20" t="s">
+      <c r="B562" s="21" t="s">
         <v>1584</v>
       </c>
-      <c r="C562" s="20" t="s">
+      <c r="C562" s="21" t="s">
         <v>1585</v>
       </c>
-      <c r="D562" s="20"/>
+      <c r="D562" s="21"/>
       <c r="E562" s="4"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="A563" s="19" t="s">
+      <c r="A563" s="20" t="s">
         <v>1586</v>
       </c>
-      <c r="B563" s="20" t="s">
+      <c r="B563" s="21" t="s">
         <v>1587</v>
       </c>
-      <c r="C563" s="20" t="s">
+      <c r="C563" s="21" t="s">
         <v>1588</v>
       </c>
-      <c r="D563" s="20"/>
+      <c r="D563" s="21"/>
       <c r="E563" s="4"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="A564" s="19" t="s">
+      <c r="A564" s="20" t="s">
         <v>1589</v>
       </c>
-      <c r="B564" s="20" t="s">
+      <c r="B564" s="21" t="s">
         <v>1590</v>
       </c>
-      <c r="C564" s="20" t="s">
+      <c r="C564" s="21" t="s">
         <v>1591</v>
       </c>
-      <c r="D564" s="20"/>
+      <c r="D564" s="21"/>
       <c r="E564" s="4"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="A565" s="19" t="s">
+      <c r="A565" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="B565" s="20" t="s">
+      <c r="B565" s="21" t="s">
         <v>1593</v>
       </c>
-      <c r="C565" s="20" t="s">
+      <c r="C565" s="21" t="s">
         <v>1594</v>
       </c>
-      <c r="D565" s="20"/>
+      <c r="D565" s="21"/>
       <c r="E565" s="4"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="A566" s="19" t="s">
+      <c r="A566" s="20" t="s">
         <v>1595</v>
       </c>
-      <c r="B566" s="20" t="s">
+      <c r="B566" s="21" t="s">
         <v>1596</v>
       </c>
-      <c r="C566" s="20" t="s">
+      <c r="C566" s="21" t="s">
         <v>1597</v>
       </c>
-      <c r="D566" s="20"/>
+      <c r="D566" s="21"/>
       <c r="E566" s="4"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="A567" s="19" t="s">
+      <c r="A567" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="B567" s="20" t="s">
+      <c r="B567" s="21" t="s">
         <v>1599</v>
       </c>
-      <c r="C567" s="20" t="s">
+      <c r="C567" s="21" t="s">
         <v>1600</v>
       </c>
-      <c r="D567" s="20"/>
+      <c r="D567" s="21"/>
       <c r="E567" s="4"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="A568" s="19" t="s">
+      <c r="A568" s="20" t="s">
         <v>1601</v>
       </c>
-      <c r="B568" s="20" t="s">
+      <c r="B568" s="21" t="s">
         <v>1602</v>
       </c>
-      <c r="C568" s="20" t="s">
+      <c r="C568" s="21" t="s">
         <v>1603</v>
       </c>
-      <c r="D568" s="20"/>
+      <c r="D568" s="21"/>
       <c r="E568" s="4"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="A569" s="19" t="s">
+      <c r="A569" s="20" t="s">
         <v>1604</v>
       </c>
-      <c r="B569" s="20" t="s">
+      <c r="B569" s="21" t="s">
         <v>1605</v>
       </c>
-      <c r="C569" s="20" t="s">
+      <c r="C569" s="21" t="s">
         <v>1606</v>
       </c>
-      <c r="D569" s="20"/>
+      <c r="D569" s="21"/>
       <c r="E569" s="4"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="A570" s="19" t="s">
+      <c r="A570" s="20" t="s">
         <v>1607</v>
       </c>
-      <c r="B570" s="20" t="s">
+      <c r="B570" s="21" t="s">
         <v>1608</v>
       </c>
-      <c r="C570" s="20" t="s">
+      <c r="C570" s="21" t="s">
         <v>1609</v>
       </c>
-      <c r="D570" s="20"/>
+      <c r="D570" s="21"/>
       <c r="E570" s="4"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="A571" s="19" t="s">
+      <c r="A571" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="B571" s="20" t="s">
+      <c r="B571" s="21" t="s">
         <v>1611</v>
       </c>
-      <c r="C571" s="20" t="s">
+      <c r="C571" s="21" t="s">
         <v>1612</v>
       </c>
-      <c r="D571" s="20"/>
+      <c r="D571" s="21"/>
       <c r="E571" s="4"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="A572" s="19" t="s">
+      <c r="A572" s="20" t="s">
         <v>1613</v>
       </c>
-      <c r="B572" s="20" t="s">
+      <c r="B572" s="21" t="s">
         <v>1614</v>
       </c>
-      <c r="C572" s="20" t="s">
+      <c r="C572" s="21" t="s">
         <v>1615</v>
       </c>
-      <c r="D572" s="20"/>
+      <c r="D572" s="21"/>
       <c r="E572" s="4"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="A573" s="19" t="s">
+      <c r="A573" s="20" t="s">
         <v>1616</v>
       </c>
-      <c r="B573" s="20" t="s">
+      <c r="B573" s="21" t="s">
         <v>1617</v>
       </c>
-      <c r="C573" s="20" t="s">
+      <c r="C573" s="21" t="s">
         <v>1618</v>
       </c>
-      <c r="D573" s="20"/>
+      <c r="D573" s="21"/>
       <c r="E573" s="4"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="A574" s="19" t="s">
+      <c r="A574" s="20" t="s">
         <v>1619</v>
       </c>
-      <c r="B574" s="20" t="s">
+      <c r="B574" s="21" t="s">
         <v>1620</v>
       </c>
-      <c r="C574" s="20" t="s">
+      <c r="C574" s="21" t="s">
         <v>1621</v>
       </c>
-      <c r="D574" s="20"/>
+      <c r="D574" s="21"/>
       <c r="E574" s="4"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="A575" s="19" t="s">
+      <c r="A575" s="20" t="s">
         <v>1622</v>
       </c>
-      <c r="B575" s="20" t="s">
+      <c r="B575" s="21" t="s">
         <v>1623</v>
       </c>
-      <c r="C575" s="20" t="s">
+      <c r="C575" s="21" t="s">
         <v>1624</v>
       </c>
-      <c r="D575" s="20"/>
+      <c r="D575" s="21"/>
       <c r="E575" s="4"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="A576" s="19" t="s">
+      <c r="A576" s="20" t="s">
         <v>1625</v>
       </c>
-      <c r="B576" s="20" t="s">
+      <c r="B576" s="21" t="s">
         <v>1626</v>
       </c>
-      <c r="C576" s="20" t="s">
+      <c r="C576" s="21" t="s">
         <v>1627</v>
       </c>
-      <c r="D576" s="20"/>
+      <c r="D576" s="21"/>
       <c r="E576" s="4"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="A577" s="19" t="s">
+      <c r="A577" s="20" t="s">
         <v>1628</v>
       </c>
-      <c r="B577" s="20" t="s">
+      <c r="B577" s="21" t="s">
         <v>1629</v>
       </c>
-      <c r="C577" s="20" t="s">
+      <c r="C577" s="21" t="s">
         <v>1630</v>
       </c>
-      <c r="D577" s="20"/>
+      <c r="D577" s="21"/>
       <c r="E577" s="4"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="A578" s="19" t="s">
+      <c r="A578" s="20" t="s">
         <v>1631</v>
       </c>
-      <c r="B578" s="20" t="s">
+      <c r="B578" s="21" t="s">
         <v>1632</v>
       </c>
-      <c r="C578" s="20" t="s">
+      <c r="C578" s="21" t="s">
         <v>1633</v>
       </c>
-      <c r="D578" s="20"/>
+      <c r="D578" s="21"/>
       <c r="E578" s="4"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="A579" s="19" t="s">
+      <c r="A579" s="20" t="s">
         <v>1634</v>
       </c>
-      <c r="B579" s="20" t="s">
+      <c r="B579" s="21" t="s">
         <v>1635</v>
       </c>
-      <c r="C579" s="20" t="s">
+      <c r="C579" s="21" t="s">
         <v>1636</v>
       </c>
-      <c r="D579" s="20"/>
+      <c r="D579" s="21"/>
       <c r="E579" s="4"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="A580" s="19" t="s">
+      <c r="A580" s="20" t="s">
         <v>1637</v>
       </c>
-      <c r="B580" s="20" t="s">
+      <c r="B580" s="21" t="s">
         <v>1638</v>
       </c>
-      <c r="C580" s="20" t="s">
+      <c r="C580" s="21" t="s">
         <v>1639</v>
       </c>
-      <c r="D580" s="20"/>
+      <c r="D580" s="21"/>
       <c r="E580" s="4"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="A581" s="19" t="s">
+      <c r="A581" s="20" t="s">
         <v>1640</v>
       </c>
-      <c r="B581" s="20" t="s">
+      <c r="B581" s="21" t="s">
         <v>1641</v>
       </c>
-      <c r="C581" s="20" t="s">
+      <c r="C581" s="21" t="s">
         <v>1642</v>
       </c>
-      <c r="D581" s="20"/>
+      <c r="D581" s="21"/>
       <c r="E581" s="4"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="A582" s="19" t="s">
+      <c r="A582" s="20" t="s">
         <v>1643</v>
       </c>
-      <c r="B582" s="20" t="s">
+      <c r="B582" s="21" t="s">
         <v>1644</v>
       </c>
-      <c r="C582" s="20" t="s">
+      <c r="C582" s="21" t="s">
         <v>1645</v>
       </c>
-      <c r="D582" s="20"/>
+      <c r="D582" s="21"/>
       <c r="E582" s="4"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="A583" s="19" t="s">
+      <c r="A583" s="20" t="s">
         <v>1646</v>
       </c>
-      <c r="B583" s="20" t="s">
+      <c r="B583" s="21" t="s">
         <v>1647</v>
       </c>
-      <c r="C583" s="20" t="s">
+      <c r="C583" s="21" t="s">
         <v>1648</v>
       </c>
-      <c r="D583" s="20"/>
+      <c r="D583" s="21"/>
       <c r="E583" s="4"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="A584" s="19" t="s">
+      <c r="A584" s="20" t="s">
         <v>1649</v>
       </c>
-      <c r="B584" s="20" t="s">
+      <c r="B584" s="21" t="s">
         <v>1650</v>
       </c>
-      <c r="C584" s="20" t="s">
+      <c r="C584" s="21" t="s">
         <v>1651</v>
       </c>
-      <c r="D584" s="20"/>
+      <c r="D584" s="21"/>
       <c r="E584" s="4"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="A585" s="19" t="s">
+      <c r="A585" s="20" t="s">
         <v>1652</v>
       </c>
-      <c r="B585" s="20" t="s">
+      <c r="B585" s="21" t="s">
         <v>1653</v>
       </c>
-      <c r="C585" s="20" t="s">
+      <c r="C585" s="21" t="s">
         <v>1654</v>
       </c>
-      <c r="D585" s="20"/>
+      <c r="D585" s="21"/>
       <c r="E585" s="4"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="A586" s="19" t="s">
+      <c r="A586" s="20" t="s">
         <v>1655</v>
       </c>
-      <c r="B586" s="20" t="s">
+      <c r="B586" s="21" t="s">
         <v>1656</v>
       </c>
-      <c r="C586" s="20" t="s">
+      <c r="C586" s="21" t="s">
         <v>1657</v>
       </c>
-      <c r="D586" s="20"/>
+      <c r="D586" s="21"/>
       <c r="E586" s="4"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="A587" s="19" t="s">
+      <c r="A587" s="20" t="s">
         <v>1658</v>
       </c>
-      <c r="B587" s="20" t="s">
+      <c r="B587" s="21" t="s">
         <v>1659</v>
       </c>
-      <c r="C587" s="20" t="s">
+      <c r="C587" s="21" t="s">
         <v>1660</v>
       </c>
-      <c r="D587" s="20"/>
+      <c r="D587" s="21"/>
       <c r="E587" s="4"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="A588" s="19" t="s">
+      <c r="A588" s="20" t="s">
         <v>1661</v>
       </c>
-      <c r="B588" s="20" t="s">
+      <c r="B588" s="21" t="s">
         <v>1662</v>
       </c>
-      <c r="C588" s="20" t="s">
+      <c r="C588" s="21" t="s">
         <v>1663</v>
       </c>
-      <c r="D588" s="20"/>
+      <c r="D588" s="21"/>
       <c r="E588" s="4"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="A589" s="19" t="s">
+      <c r="A589" s="20" t="s">
         <v>1664</v>
       </c>
-      <c r="B589" s="20" t="s">
+      <c r="B589" s="21" t="s">
         <v>1665</v>
       </c>
-      <c r="C589" s="20" t="s">
+      <c r="C589" s="21" t="s">
         <v>1666</v>
       </c>
-      <c r="D589" s="20"/>
+      <c r="D589" s="21"/>
       <c r="E589" s="4"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="A590" s="19" t="s">
+      <c r="A590" s="20" t="s">
         <v>1667</v>
       </c>
-      <c r="B590" s="20" t="s">
+      <c r="B590" s="21" t="s">
         <v>1668</v>
       </c>
-      <c r="C590" s="20" t="s">
+      <c r="C590" s="21" t="s">
         <v>1669</v>
       </c>
-      <c r="D590" s="20"/>
+      <c r="D590" s="21"/>
       <c r="E590" s="4"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="A591" s="24" t="s">
+      <c r="A591" s="25" t="s">
         <v>1670</v>
       </c>
-      <c r="B591" s="20" t="s">
+      <c r="B591" s="21" t="s">
         <v>1671</v>
       </c>
-      <c r="C591" s="20" t="s">
+      <c r="C591" s="21" t="s">
         <v>1672</v>
       </c>
-      <c r="D591" s="20"/>
+      <c r="D591" s="21"/>
       <c r="E591" s="4"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="A592" s="19" t="s">
+      <c r="A592" s="20" t="s">
         <v>1673</v>
       </c>
-      <c r="B592" s="20" t="s">
+      <c r="B592" s="21" t="s">
         <v>1674</v>
       </c>
-      <c r="C592" s="20" t="s">
+      <c r="C592" s="21" t="s">
         <v>1675</v>
       </c>
-      <c r="D592" s="20"/>
+      <c r="D592" s="21"/>
       <c r="E592" s="4"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="A593" s="19" t="s">
+      <c r="A593" s="20" t="s">
         <v>1676</v>
       </c>
-      <c r="B593" s="20" t="s">
+      <c r="B593" s="21" t="s">
         <v>1677</v>
       </c>
-      <c r="C593" s="20" t="s">
+      <c r="C593" s="21" t="s">
         <v>1678</v>
       </c>
-      <c r="D593" s="20"/>
+      <c r="D593" s="21"/>
       <c r="E593" s="4"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="A594" s="24" t="s">
+      <c r="A594" s="25" t="s">
         <v>1679</v>
       </c>
-      <c r="B594" s="20" t="s">
+      <c r="B594" s="21" t="s">
         <v>1680</v>
       </c>
-      <c r="C594" s="20" t="s">
+      <c r="C594" s="21" t="s">
         <v>1681</v>
       </c>
-      <c r="D594" s="20"/>
+      <c r="D594" s="21"/>
       <c r="E594" s="4"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="A595" s="19" t="s">
+      <c r="A595" s="20" t="s">
         <v>1682</v>
       </c>
-      <c r="B595" s="20" t="s">
+      <c r="B595" s="21" t="s">
         <v>1683</v>
       </c>
-      <c r="C595" s="20" t="s">
+      <c r="C595" s="21" t="s">
         <v>1684</v>
       </c>
-      <c r="D595" s="20"/>
+      <c r="D595" s="21"/>
       <c r="E595" s="4"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="A596" s="19" t="s">
+      <c r="A596" s="20" t="s">
         <v>1685</v>
       </c>
-      <c r="B596" s="20" t="s">
+      <c r="B596" s="21" t="s">
         <v>1686</v>
       </c>
-      <c r="C596" s="20" t="s">
+      <c r="C596" s="21" t="s">
         <v>1687</v>
       </c>
-      <c r="D596" s="20"/>
+      <c r="D596" s="21"/>
       <c r="E596" s="4"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="A597" s="19" t="s">
+      <c r="A597" s="20" t="s">
         <v>1688</v>
       </c>
-      <c r="B597" s="20" t="s">
+      <c r="B597" s="21" t="s">
         <v>1689</v>
       </c>
-      <c r="C597" s="20" t="s">
+      <c r="C597" s="21" t="s">
         <v>1690</v>
       </c>
-      <c r="D597" s="20"/>
+      <c r="D597" s="21"/>
       <c r="E597" s="4"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="A598" s="19" t="s">
+      <c r="A598" s="20" t="s">
         <v>1691</v>
       </c>
-      <c r="B598" s="20" t="s">
+      <c r="B598" s="21" t="s">
         <v>1692</v>
       </c>
-      <c r="C598" s="20" t="s">
+      <c r="C598" s="21" t="s">
         <v>1693</v>
       </c>
-      <c r="D598" s="20"/>
+      <c r="D598" s="21"/>
       <c r="E598" s="4"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="A599" s="24" t="s">
+      <c r="A599" s="25" t="s">
         <v>1694</v>
       </c>
-      <c r="B599" s="20" t="s">
+      <c r="B599" s="21" t="s">
         <v>1695</v>
       </c>
-      <c r="C599" s="20" t="s">
+      <c r="C599" s="21" t="s">
         <v>1696</v>
       </c>
-      <c r="D599" s="20"/>
+      <c r="D599" s="21"/>
       <c r="E599" s="4"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="A600" s="19" t="s">
+      <c r="A600" s="20" t="s">
         <v>1697</v>
       </c>
-      <c r="B600" s="20" t="s">
+      <c r="B600" s="21" t="s">
         <v>1698</v>
       </c>
-      <c r="C600" s="20" t="s">
+      <c r="C600" s="21" t="s">
         <v>1699</v>
       </c>
-      <c r="D600" s="20"/>
+      <c r="D600" s="21"/>
       <c r="E600" s="4"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="A601" s="19" t="s">
+      <c r="A601" s="20" t="s">
         <v>1700</v>
       </c>
-      <c r="B601" s="20" t="s">
+      <c r="B601" s="21" t="s">
         <v>1701</v>
       </c>
-      <c r="C601" s="20" t="s">
+      <c r="C601" s="21" t="s">
         <v>1702</v>
       </c>
-      <c r="D601" s="20"/>
+      <c r="D601" s="21"/>
       <c r="E601" s="4"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="A602" s="19" t="s">
+      <c r="A602" s="20" t="s">
         <v>1703</v>
       </c>
-      <c r="B602" s="20" t="s">
+      <c r="B602" s="21" t="s">
         <v>1704</v>
       </c>
-      <c r="C602" s="20" t="s">
+      <c r="C602" s="21" t="s">
         <v>1705</v>
       </c>
-      <c r="D602" s="20"/>
+      <c r="D602" s="21"/>
       <c r="E602" s="4"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="A603" s="19" t="s">
+      <c r="A603" s="20" t="s">
         <v>1706</v>
       </c>
-      <c r="B603" s="20" t="s">
+      <c r="B603" s="21" t="s">
         <v>1707</v>
       </c>
-      <c r="C603" s="20" t="s">
+      <c r="C603" s="21" t="s">
         <v>1708</v>
       </c>
-      <c r="D603" s="20"/>
+      <c r="D603" s="21"/>
       <c r="E603" s="4"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="A604" s="19" t="s">
+      <c r="A604" s="20" t="s">
         <v>1709</v>
       </c>
-      <c r="B604" s="20" t="s">
+      <c r="B604" s="21" t="s">
         <v>1710</v>
       </c>
-      <c r="C604" s="20" t="s">
+      <c r="C604" s="21" t="s">
         <v>1711</v>
       </c>
-      <c r="D604" s="20"/>
+      <c r="D604" s="21"/>
       <c r="E604" s="4"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="A605" s="25" t="s">
+      <c r="A605" s="26" t="s">
         <v>1712</v>
       </c>
-      <c r="B605" s="20" t="s">
+      <c r="B605" s="21" t="s">
         <v>1713</v>
       </c>
-      <c r="C605" s="20" t="s">
+      <c r="C605" s="21" t="s">
         <v>1714</v>
       </c>
-      <c r="D605" s="20"/>
+      <c r="D605" s="21"/>
       <c r="E605" s="4"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="A606" s="19" t="s">
+      <c r="A606" s="20" t="s">
         <v>1715</v>
       </c>
-      <c r="B606" s="20" t="s">
+      <c r="B606" s="21" t="s">
         <v>1716</v>
       </c>
-      <c r="C606" s="20" t="s">
+      <c r="C606" s="21" t="s">
         <v>1717</v>
       </c>
-      <c r="D606" s="20"/>
+      <c r="D606" s="21"/>
       <c r="E606" s="4"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="A607" s="19" t="s">
+      <c r="A607" s="20" t="s">
         <v>1718</v>
       </c>
-      <c r="B607" s="20" t="s">
+      <c r="B607" s="21" t="s">
         <v>1719</v>
       </c>
-      <c r="C607" s="20" t="s">
+      <c r="C607" s="21" t="s">
         <v>1720</v>
       </c>
-      <c r="D607" s="20"/>
+      <c r="D607" s="21"/>
       <c r="E607" s="4"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="A608" s="19" t="s">
+      <c r="A608" s="20" t="s">
         <v>1721</v>
       </c>
-      <c r="B608" s="20" t="s">
+      <c r="B608" s="21" t="s">
         <v>1722</v>
       </c>
-      <c r="C608" s="20" t="s">
+      <c r="C608" s="21" t="s">
         <v>1723</v>
       </c>
-      <c r="D608" s="20"/>
+      <c r="D608" s="21"/>
       <c r="E608" s="4"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="A609" s="19" t="s">
+      <c r="A609" s="20" t="s">
         <v>1724</v>
       </c>
-      <c r="B609" s="20" t="s">
+      <c r="B609" s="21" t="s">
         <v>1725</v>
       </c>
-      <c r="C609" s="20" t="s">
+      <c r="C609" s="21" t="s">
         <v>1726</v>
       </c>
-      <c r="D609" s="20"/>
+      <c r="D609" s="21"/>
       <c r="E609" s="4"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="A610" s="19" t="s">
+      <c r="A610" s="20" t="s">
         <v>1727</v>
       </c>
-      <c r="B610" s="20" t="s">
+      <c r="B610" s="21" t="s">
         <v>1728</v>
       </c>
-      <c r="C610" s="20" t="s">
+      <c r="C610" s="21" t="s">
         <v>1729</v>
       </c>
-      <c r="D610" s="20"/>
+      <c r="D610" s="21"/>
       <c r="E610" s="4"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="A611" s="19" t="s">
+      <c r="A611" s="20" t="s">
         <v>1730</v>
       </c>
-      <c r="B611" s="20" t="s">
+      <c r="B611" s="21" t="s">
         <v>1731</v>
       </c>
-      <c r="C611" s="20" t="s">
+      <c r="C611" s="21" t="s">
         <v>1732</v>
       </c>
-      <c r="D611" s="20"/>
+      <c r="D611" s="21"/>
       <c r="E611" s="4"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="A612" s="19" t="s">
+      <c r="A612" s="20" t="s">
         <v>1733</v>
       </c>
-      <c r="B612" s="20" t="s">
+      <c r="B612" s="21" t="s">
         <v>1734</v>
       </c>
-      <c r="C612" s="20" t="s">
+      <c r="C612" s="21" t="s">
         <v>1735</v>
       </c>
-      <c r="D612" s="20"/>
+      <c r="D612" s="21"/>
       <c r="E612" s="4"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="A613" s="19" t="s">
+      <c r="A613" s="20" t="s">
         <v>1736</v>
       </c>
-      <c r="B613" s="20" t="s">
+      <c r="B613" s="21" t="s">
         <v>1737</v>
       </c>
-      <c r="C613" s="20" t="s">
+      <c r="C613" s="21" t="s">
         <v>1738</v>
       </c>
-      <c r="D613" s="20"/>
+      <c r="D613" s="21"/>
       <c r="E613" s="4"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="A614" s="19" t="s">
+      <c r="A614" s="20" t="s">
         <v>1739</v>
       </c>
-      <c r="B614" s="20" t="s">
+      <c r="B614" s="21" t="s">
         <v>1740</v>
       </c>
-      <c r="C614" s="20" t="s">
+      <c r="C614" s="21" t="s">
         <v>1741</v>
       </c>
-      <c r="D614" s="20"/>
+      <c r="D614" s="21"/>
       <c r="E614" s="4"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="A615" s="19" t="s">
+      <c r="A615" s="20" t="s">
         <v>1742</v>
       </c>
-      <c r="B615" s="20" t="s">
+      <c r="B615" s="21" t="s">
         <v>1743</v>
       </c>
-      <c r="C615" s="20" t="s">
+      <c r="C615" s="21" t="s">
         <v>1744</v>
       </c>
-      <c r="D615" s="20"/>
+      <c r="D615" s="21"/>
       <c r="E615" s="4"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="A616" s="19" t="s">
+      <c r="A616" s="20" t="s">
         <v>1745</v>
       </c>
-      <c r="B616" s="20" t="s">
+      <c r="B616" s="21" t="s">
         <v>1746</v>
       </c>
-      <c r="C616" s="20" t="s">
+      <c r="C616" s="21" t="s">
         <v>1747</v>
       </c>
-      <c r="D616" s="20"/>
+      <c r="D616" s="21"/>
       <c r="E616" s="4"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="A617" s="19" t="s">
+      <c r="A617" s="20" t="s">
         <v>1748</v>
       </c>
-      <c r="B617" s="20" t="s">
+      <c r="B617" s="21" t="s">
         <v>1749</v>
       </c>
-      <c r="C617" s="20" t="s">
+      <c r="C617" s="21" t="s">
         <v>1750</v>
       </c>
-      <c r="D617" s="20"/>
+      <c r="D617" s="21"/>
       <c r="E617" s="4"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="A618" s="26" t="s">
+      <c r="A618" s="27" t="s">
         <v>1751</v>
       </c>
       <c r="B618" s="12" t="s">
@@ -14165,7 +14181,7 @@
       <c r="E618" s="4"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="A619" s="26" t="s">
+      <c r="A619" s="27" t="s">
         <v>1754</v>
       </c>
       <c r="B619" s="12" t="s">
@@ -14178,7 +14194,7 @@
       <c r="E619" s="4"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="A620" s="27" t="s">
+      <c r="A620" s="28" t="s">
         <v>1757</v>
       </c>
       <c r="B620" s="12" t="s">
@@ -14191,7 +14207,7 @@
       <c r="E620" s="4"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="A621" s="26" t="s">
+      <c r="A621" s="27" t="s">
         <v>1760</v>
       </c>
       <c r="B621" s="12" t="s">
@@ -14204,7 +14220,7 @@
       <c r="E621" s="4"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="A622" s="26" t="s">
+      <c r="A622" s="27" t="s">
         <v>1763</v>
       </c>
       <c r="B622" s="12" t="s">
@@ -14217,7 +14233,7 @@
       <c r="E622" s="4"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="A623" s="26" t="s">
+      <c r="A623" s="27" t="s">
         <v>1766</v>
       </c>
       <c r="B623" s="12" t="s">
@@ -14230,7 +14246,7 @@
       <c r="E623" s="4"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="A624" s="26" t="s">
+      <c r="A624" s="27" t="s">
         <v>1769</v>
       </c>
       <c r="B624" s="12" t="s">
@@ -14243,7 +14259,7 @@
       <c r="E624" s="4"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="A625" s="26" t="s">
+      <c r="A625" s="27" t="s">
         <v>1772</v>
       </c>
       <c r="B625" s="12" t="s">
@@ -14256,7 +14272,7 @@
       <c r="E625" s="4"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="A626" s="26" t="s">
+      <c r="A626" s="27" t="s">
         <v>1775</v>
       </c>
       <c r="B626" s="12" t="s">
@@ -14269,7 +14285,7 @@
       <c r="E626" s="4"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="A627" s="26" t="s">
+      <c r="A627" s="27" t="s">
         <v>1778</v>
       </c>
       <c r="B627" s="12" t="s">
@@ -14282,7 +14298,7 @@
       <c r="E627" s="4"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="A628" s="26" t="s">
+      <c r="A628" s="27" t="s">
         <v>1781</v>
       </c>
       <c r="B628" s="12" t="s">
@@ -14295,7 +14311,7 @@
       <c r="E628" s="4"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="A629" s="26" t="s">
+      <c r="A629" s="27" t="s">
         <v>1784</v>
       </c>
       <c r="B629" s="12" t="s">
@@ -14308,7 +14324,7 @@
       <c r="E629" s="4"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="A630" s="26" t="s">
+      <c r="A630" s="27" t="s">
         <v>1787</v>
       </c>
       <c r="B630" s="12" t="s">
@@ -14321,7 +14337,7 @@
       <c r="E630" s="4"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="A631" s="26" t="s">
+      <c r="A631" s="27" t="s">
         <v>1790</v>
       </c>
       <c r="B631" s="12" t="s">
@@ -14334,7 +14350,7 @@
       <c r="E631" s="4"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="A632" s="26" t="s">
+      <c r="A632" s="27" t="s">
         <v>1793</v>
       </c>
       <c r="B632" s="12" t="s">
@@ -14347,7 +14363,7 @@
       <c r="E632" s="4"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="A633" s="26" t="s">
+      <c r="A633" s="27" t="s">
         <v>1796</v>
       </c>
       <c r="B633" s="12" t="s">
@@ -14360,7 +14376,7 @@
       <c r="E633" s="4"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="A634" s="26" t="s">
+      <c r="A634" s="27" t="s">
         <v>1799</v>
       </c>
       <c r="B634" s="12" t="s">
@@ -14373,7 +14389,7 @@
       <c r="E634" s="4"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="A635" s="26" t="s">
+      <c r="A635" s="27" t="s">
         <v>1802</v>
       </c>
       <c r="B635" s="12" t="s">
@@ -14386,7 +14402,7 @@
       <c r="E635" s="4"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="A636" s="26" t="s">
+      <c r="A636" s="27" t="s">
         <v>1805</v>
       </c>
       <c r="B636" s="12" t="s">
@@ -14399,7 +14415,7 @@
       <c r="E636" s="4"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="A637" s="26" t="s">
+      <c r="A637" s="27" t="s">
         <v>1808</v>
       </c>
       <c r="B637" s="12" t="s">
@@ -14412,7 +14428,7 @@
       <c r="E637" s="4"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="A638" s="26" t="s">
+      <c r="A638" s="27" t="s">
         <v>1811</v>
       </c>
       <c r="B638" s="12" t="s">
@@ -14425,7 +14441,7 @@
       <c r="E638" s="4"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="A639" s="26" t="s">
+      <c r="A639" s="27" t="s">
         <v>1814</v>
       </c>
       <c r="B639" s="12" t="s">
@@ -14438,7 +14454,7 @@
       <c r="E639" s="4"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="A640" s="26" t="s">
+      <c r="A640" s="27" t="s">
         <v>1817</v>
       </c>
       <c r="B640" s="12" t="s">
@@ -14451,7 +14467,7 @@
       <c r="E640" s="4"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="A641" s="26" t="s">
+      <c r="A641" s="27" t="s">
         <v>1820</v>
       </c>
       <c r="B641" s="12" t="s">
@@ -14464,7 +14480,7 @@
       <c r="E641" s="4"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="A642" s="26" t="s">
+      <c r="A642" s="27" t="s">
         <v>1823</v>
       </c>
       <c r="B642" s="12" t="s">
@@ -14477,21 +14493,21 @@
       <c r="E642" s="4"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="A643" s="28" t="s">
+      <c r="A643" s="29" t="s">
         <v>1826</v>
       </c>
-      <c r="B643" s="29" t="s">
+      <c r="B643" s="30" t="s">
         <v>1482</v>
       </c>
-      <c r="C643" s="29" t="s">
+      <c r="C643" s="30" t="s">
         <v>1483</v>
       </c>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="A644" s="26" t="s">
+      <c r="A644" s="27" t="s">
         <v>1827</v>
       </c>
-      <c r="B644" s="29" t="s">
+      <c r="B644" s="30" t="s">
         <v>1828</v>
       </c>
       <c r="C644" s="12" t="s">
@@ -14499,7 +14515,7 @@
       </c>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="A645" s="26" t="s">
+      <c r="A645" s="27" t="s">
         <v>1830</v>
       </c>
       <c r="B645" s="12" t="s">
@@ -14510,7 +14526,7 @@
       </c>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="A646" s="26" t="s">
+      <c r="A646" s="27" t="s">
         <v>1833</v>
       </c>
       <c r="B646" s="12" t="s">
@@ -14521,7 +14537,7 @@
       </c>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="A647" s="26" t="s">
+      <c r="A647" s="27" t="s">
         <v>1836</v>
       </c>
       <c r="B647" s="12" t="s">
@@ -14532,7 +14548,7 @@
       </c>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="A648" s="26" t="s">
+      <c r="A648" s="27" t="s">
         <v>1839</v>
       </c>
       <c r="B648" s="12" t="s">
@@ -14543,447 +14559,447 @@
       </c>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="A649" s="22" t="s">
+      <c r="A649" s="23" t="s">
         <v>1842</v>
       </c>
-      <c r="B649" s="23" t="s">
+      <c r="B649" s="24" t="s">
         <v>1843</v>
       </c>
-      <c r="C649" s="23" t="s">
+      <c r="C649" s="24" t="s">
         <v>1844</v>
       </c>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="A650" s="22" t="s">
+      <c r="A650" s="23" t="s">
         <v>1845</v>
       </c>
-      <c r="B650" s="23" t="s">
+      <c r="B650" s="24" t="s">
         <v>1846</v>
       </c>
-      <c r="C650" s="23" t="s">
+      <c r="C650" s="24" t="s">
         <v>1847</v>
       </c>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="A651" s="22" t="s">
+      <c r="A651" s="23" t="s">
         <v>1848</v>
       </c>
-      <c r="B651" s="23" t="s">
+      <c r="B651" s="24" t="s">
         <v>1849</v>
       </c>
-      <c r="C651" s="23" t="s">
+      <c r="C651" s="24" t="s">
         <v>1850</v>
       </c>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="A652" s="22" t="s">
+      <c r="A652" s="23" t="s">
         <v>1851</v>
       </c>
-      <c r="B652" s="23" t="s">
+      <c r="B652" s="24" t="s">
         <v>1584</v>
       </c>
-      <c r="C652" s="23" t="s">
+      <c r="C652" s="24" t="s">
         <v>1585</v>
       </c>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="A653" s="30" t="s">
+      <c r="A653" s="31" t="s">
         <v>1852</v>
       </c>
-      <c r="B653" s="23" t="s">
+      <c r="B653" s="24" t="s">
         <v>1853</v>
       </c>
-      <c r="C653" s="31" t="str">
+      <c r="C653" s="32" t="str">
         <f t="shared" ref="C653:C685" si="1">CONCATENATE("&amp;", B653)</f>
         <v>&amp;Improve connection with community</v>
       </c>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="A654" s="30" t="s">
+      <c r="A654" s="31" t="s">
         <v>1854</v>
       </c>
-      <c r="B654" s="23" t="s">
+      <c r="B654" s="24" t="s">
         <v>1855</v>
       </c>
-      <c r="C654" s="31" t="str">
+      <c r="C654" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Improve connection with family</v>
       </c>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="A655" s="30" t="s">
+      <c r="A655" s="31" t="s">
         <v>1856</v>
       </c>
-      <c r="B655" s="23" t="s">
+      <c r="B655" s="24" t="s">
         <v>1857</v>
       </c>
-      <c r="C655" s="31" t="str">
+      <c r="C655" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Be more social with others</v>
       </c>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="A656" s="30" t="s">
+      <c r="A656" s="31" t="s">
         <v>1858</v>
       </c>
-      <c r="B656" s="23" t="s">
+      <c r="B656" s="24" t="s">
         <v>1859</v>
       </c>
-      <c r="C656" s="31" t="str">
+      <c r="C656" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Obtain additional food supplies</v>
       </c>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="A657" s="30" t="s">
+      <c r="A657" s="31" t="s">
         <v>1860</v>
       </c>
-      <c r="B657" s="23" t="s">
+      <c r="B657" s="24" t="s">
         <v>1861</v>
       </c>
-      <c r="C657" s="31" t="str">
+      <c r="C657" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Have a balanced diet</v>
       </c>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="A658" s="30" t="s">
+      <c r="A658" s="31" t="s">
         <v>1862</v>
       </c>
-      <c r="B658" s="23" t="s">
+      <c r="B658" s="24" t="s">
         <v>1863</v>
       </c>
-      <c r="C658" s="31" t="str">
+      <c r="C658" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve counselling</v>
       </c>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="A659" s="30" t="s">
+      <c r="A659" s="31" t="s">
         <v>1864</v>
       </c>
-      <c r="B659" s="23" t="s">
+      <c r="B659" s="24" t="s">
         <v>1865</v>
       </c>
-      <c r="C659" s="31" t="str">
+      <c r="C659" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve medication</v>
       </c>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="A660" s="30" t="s">
+      <c r="A660" s="31" t="s">
         <v>1866</v>
       </c>
-      <c r="B660" s="23" t="s">
+      <c r="B660" s="24" t="s">
         <v>1865</v>
       </c>
-      <c r="C660" s="31" t="str">
+      <c r="C660" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve medication</v>
       </c>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="A661" s="30" t="s">
+      <c r="A661" s="31" t="s">
         <v>1867</v>
       </c>
-      <c r="B661" s="23" t="s">
+      <c r="B661" s="24" t="s">
         <v>1868</v>
       </c>
-      <c r="C661" s="31" t="str">
+      <c r="C661" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve wheelchair</v>
       </c>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="A662" s="30" t="s">
+      <c r="A662" s="31" t="s">
         <v>1869</v>
       </c>
-      <c r="B662" s="23" t="s">
+      <c r="B662" s="24" t="s">
         <v>1870</v>
       </c>
-      <c r="C662" s="31" t="str">
+      <c r="C662" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve crutches</v>
       </c>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="A663" s="30" t="s">
+      <c r="A663" s="31" t="s">
         <v>1871</v>
       </c>
-      <c r="B663" s="23" t="s">
+      <c r="B663" s="24" t="s">
         <v>1872</v>
       </c>
-      <c r="C663" s="31" t="str">
+      <c r="C663" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Improve personal hygeine</v>
       </c>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="A664" s="30" t="s">
+      <c r="A664" s="31" t="s">
         <v>1873</v>
       </c>
-      <c r="B664" s="23" t="s">
+      <c r="B664" s="24" t="s">
         <v>1874</v>
       </c>
-      <c r="C664" s="31" t="str">
+      <c r="C664" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Recieve technical training</v>
       </c>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="A665" s="30" t="s">
+      <c r="A665" s="31" t="s">
         <v>1875</v>
       </c>
-      <c r="B665" s="23" t="s">
+      <c r="B665" s="24" t="s">
         <v>1876</v>
       </c>
-      <c r="C665" s="31" t="str">
+      <c r="C665" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Enroll in a skills development course</v>
       </c>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="A666" s="30" t="s">
+      <c r="A666" s="31" t="s">
         <v>1877</v>
       </c>
-      <c r="B666" s="23" t="s">
+      <c r="B666" s="24" t="s">
         <v>1878</v>
       </c>
-      <c r="C666" s="31" t="str">
+      <c r="C666" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Achieved</v>
       </c>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="A667" s="30" t="s">
+      <c r="A667" s="31" t="s">
         <v>1879</v>
       </c>
-      <c r="B667" s="23" t="s">
+      <c r="B667" s="24" t="s">
         <v>1880</v>
       </c>
-      <c r="C667" s="31" t="str">
+      <c r="C667" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;In progress</v>
       </c>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="A668" s="30" t="s">
+      <c r="A668" s="31" t="s">
         <v>1881</v>
       </c>
-      <c r="B668" s="23" t="s">
+      <c r="B668" s="24" t="s">
         <v>1882</v>
       </c>
-      <c r="C668" s="31" t="str">
+      <c r="C668" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Not Achieved</v>
       </c>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="A669" s="30" t="s">
+      <c r="A669" s="31" t="s">
         <v>1883</v>
       </c>
-      <c r="B669" s="23" t="s">
+      <c r="B669" s="24" t="s">
         <v>1884</v>
       </c>
-      <c r="C669" s="31" t="str">
+      <c r="C669" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="A670" s="30" t="s">
+      <c r="A670" s="31" t="s">
         <v>1885</v>
       </c>
-      <c r="B670" s="23" t="s">
+      <c r="B670" s="24" t="s">
         <v>1878</v>
       </c>
-      <c r="C670" s="31" t="str">
+      <c r="C670" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Achieved</v>
       </c>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="A671" s="30" t="s">
+      <c r="A671" s="31" t="s">
         <v>1886</v>
       </c>
-      <c r="B671" s="23" t="s">
+      <c r="B671" s="24" t="s">
         <v>1880</v>
       </c>
-      <c r="C671" s="31" t="str">
+      <c r="C671" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;In progress</v>
       </c>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="A672" s="30" t="s">
+      <c r="A672" s="31" t="s">
         <v>1887</v>
       </c>
-      <c r="B672" s="23" t="s">
+      <c r="B672" s="24" t="s">
         <v>1882</v>
       </c>
-      <c r="C672" s="31" t="str">
+      <c r="C672" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Not Achieved</v>
       </c>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="A673" s="30" t="s">
+      <c r="A673" s="31" t="s">
         <v>1888</v>
       </c>
-      <c r="B673" s="23" t="s">
+      <c r="B673" s="24" t="s">
         <v>1884</v>
       </c>
-      <c r="C673" s="31" t="str">
+      <c r="C673" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="A674" s="30" t="s">
+      <c r="A674" s="31" t="s">
         <v>1889</v>
       </c>
-      <c r="B674" s="23" t="s">
+      <c r="B674" s="24" t="s">
         <v>1878</v>
       </c>
-      <c r="C674" s="31" t="str">
+      <c r="C674" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Achieved</v>
       </c>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="A675" s="30" t="s">
+      <c r="A675" s="31" t="s">
         <v>1890</v>
       </c>
-      <c r="B675" s="23" t="s">
+      <c r="B675" s="24" t="s">
         <v>1880</v>
       </c>
-      <c r="C675" s="31" t="str">
+      <c r="C675" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;In progress</v>
       </c>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="A676" s="30" t="s">
+      <c r="A676" s="31" t="s">
         <v>1891</v>
       </c>
-      <c r="B676" s="23" t="s">
+      <c r="B676" s="24" t="s">
         <v>1882</v>
       </c>
-      <c r="C676" s="31" t="str">
+      <c r="C676" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Not Achieved</v>
       </c>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="A677" s="30" t="s">
+      <c r="A677" s="31" t="s">
         <v>1892</v>
       </c>
-      <c r="B677" s="23" t="s">
+      <c r="B677" s="24" t="s">
         <v>1884</v>
       </c>
-      <c r="C677" s="31" t="str">
+      <c r="C677" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="A678" s="30" t="s">
+      <c r="A678" s="31" t="s">
         <v>1893</v>
       </c>
-      <c r="B678" s="23" t="s">
+      <c r="B678" s="24" t="s">
         <v>1878</v>
       </c>
-      <c r="C678" s="31" t="str">
+      <c r="C678" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Achieved</v>
       </c>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="A679" s="30" t="s">
+      <c r="A679" s="31" t="s">
         <v>1894</v>
       </c>
-      <c r="B679" s="23" t="s">
+      <c r="B679" s="24" t="s">
         <v>1880</v>
       </c>
-      <c r="C679" s="31" t="str">
+      <c r="C679" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;In progress</v>
       </c>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="A680" s="30" t="s">
+      <c r="A680" s="31" t="s">
         <v>1895</v>
       </c>
-      <c r="B680" s="23" t="s">
+      <c r="B680" s="24" t="s">
         <v>1882</v>
       </c>
-      <c r="C680" s="31" t="str">
+      <c r="C680" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Not Achieved</v>
       </c>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="A681" s="30" t="s">
+      <c r="A681" s="31" t="s">
         <v>1896</v>
       </c>
-      <c r="B681" s="23" t="s">
+      <c r="B681" s="24" t="s">
         <v>1884</v>
       </c>
-      <c r="C681" s="31" t="str">
+      <c r="C681" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="A682" s="30" t="s">
+      <c r="A682" s="31" t="s">
         <v>1897</v>
       </c>
-      <c r="B682" s="23" t="s">
+      <c r="B682" s="24" t="s">
         <v>1878</v>
       </c>
-      <c r="C682" s="31" t="str">
+      <c r="C682" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Achieved</v>
       </c>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="A683" s="30" t="s">
+      <c r="A683" s="31" t="s">
         <v>1898</v>
       </c>
-      <c r="B683" s="23" t="s">
+      <c r="B683" s="24" t="s">
         <v>1880</v>
       </c>
-      <c r="C683" s="31" t="str">
+      <c r="C683" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;In progress</v>
       </c>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="A684" s="30" t="s">
+      <c r="A684" s="31" t="s">
         <v>1899</v>
       </c>
-      <c r="B684" s="23" t="s">
+      <c r="B684" s="24" t="s">
         <v>1882</v>
       </c>
-      <c r="C684" s="31" t="str">
+      <c r="C684" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;Not Achieved</v>
       </c>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="A685" s="30" t="s">
+      <c r="A685" s="31" t="s">
         <v>1900</v>
       </c>
-      <c r="B685" s="23" t="s">
+      <c r="B685" s="24" t="s">
         <v>1884</v>
       </c>
-      <c r="C685" s="31" t="str">
+      <c r="C685" s="32" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="A686" s="26" t="s">
+      <c r="A686" s="27" t="s">
         <v>1901</v>
       </c>
       <c r="B686" s="12" t="s">
@@ -14993,7 +15009,17 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1">
+      <c r="A687" s="23" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B687" s="12" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C687" s="12" t="s">
+        <v>1906</v>
+      </c>
+    </row>
     <row r="688" ht="15.75" customHeight="1"/>
     <row r="689" ht="15.75" customHeight="1"/>
     <row r="690" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
translations: add DataGrid label translations
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="1908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="1914">
   <si>
     <t>Key</t>
   </si>
@@ -5747,13 +5747,31 @@
   </si>
   <si>
     <t>&amp;Filter by Referral Types</t>
+  </si>
+  <si>
+    <t>general.dataGridLabelRowsPerPage</t>
+  </si>
+  <si>
+    <t>Rows per page:</t>
+  </si>
+  <si>
+    <t>&amp;Rows per page:</t>
+  </si>
+  <si>
+    <t>general.dataGridLabelDisplayedRows</t>
+  </si>
+  <si>
+    <t>{{from}}–{{to}} of {{count}}</t>
+  </si>
+  <si>
+    <t>&amp;{{from}}–{{to}} of {{count}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -5790,6 +5808,12 @@
       <sz val="11.0"/>
       <color rgb="FF17191C"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -5836,7 +5860,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5916,6 +5940,16 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -14990,41 +15024,61 @@
       </c>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="A685" s="31" t="s">
+      <c r="A685" s="33" t="s">
         <v>1901</v>
       </c>
-      <c r="B685" s="24" t="s">
+      <c r="B685" s="34" t="s">
         <v>1885</v>
       </c>
-      <c r="C685" s="32" t="str">
+      <c r="C685" s="35" t="str">
         <f t="shared" si="1"/>
         <v>&amp;No goals</v>
       </c>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="A686" s="27" t="s">
+      <c r="A686" s="36" t="s">
         <v>1902</v>
       </c>
-      <c r="B686" s="12" t="s">
+      <c r="B686" s="34" t="s">
         <v>1903</v>
       </c>
-      <c r="C686" s="12" t="s">
+      <c r="C686" s="34" t="s">
         <v>1904</v>
       </c>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="A687" s="23" t="s">
+      <c r="A687" s="36" t="s">
         <v>1905</v>
       </c>
-      <c r="B687" s="12" t="s">
+      <c r="B687" s="34" t="s">
         <v>1906</v>
       </c>
-      <c r="C687" s="12" t="s">
+      <c r="C687" s="34" t="s">
         <v>1907</v>
       </c>
     </row>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1">
+      <c r="A688" s="36" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B688" s="34" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C688" s="34" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="689" ht="19.5" customHeight="1">
+      <c r="A689" s="36" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B689" s="24" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C689" s="24" t="s">
+        <v>1913</v>
+      </c>
+    </row>
     <row r="690" ht="15.75" customHeight="1"/>
     <row r="691" ht="15.75" customHeight="1"/>
     <row r="692" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added a hover note with translation for referral details
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1926">
   <si>
     <t>Key</t>
   </si>
@@ -5792,6 +5792,15 @@
   </si>
   <si>
     <t>&amp;All</t>
+  </si>
+  <si>
+    <t>referral.hoverDetails</t>
+  </si>
+  <si>
+    <t>Hover over the details to see more information about each referral.</t>
+  </si>
+  <si>
+    <t>&amp;Hover over the details to see more information about each referral.</t>
   </si>
 </sst>
 </file>
@@ -15139,7 +15148,17 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1">
+      <c r="A693" s="36" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B693" s="24" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C693" s="24" t="s">
+        <v>1925</v>
+      </c>
+    </row>
     <row r="694" ht="15.75" customHeight="1"/>
     <row r="695" ht="15.75" customHeight="1"/>
     <row r="696" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updated follow up stats and new client stats ui
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1962">
   <si>
     <t>Key</t>
   </si>
@@ -5792,6 +5792,123 @@
   </si>
   <si>
     <t>&amp;All</t>
+  </si>
+  <si>
+    <t>referral.hoverDetails</t>
+  </si>
+  <si>
+    <t>Hover over the details to see more information about each referral.</t>
+  </si>
+  <si>
+    <t>&amp;Hover over the details to see more information about each referral.</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpFAdult</t>
+  </si>
+  <si>
+    <t>Total Followed Up Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpMAdult</t>
+  </si>
+  <si>
+    <t>Total Followed Up Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpFChild</t>
+  </si>
+  <si>
+    <t>Total Followed Up Female Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Female Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpMChild</t>
+  </si>
+  <si>
+    <t>Total Followed Up Male Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Male Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.followUpVisits</t>
+  </si>
+  <si>
+    <t>Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.newClients</t>
+  </si>
+  <si>
+    <t>New Clients:</t>
+  </si>
+  <si>
+    <t>&amp;New Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewFAdult</t>
+  </si>
+  <si>
+    <t>Total New Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewMAdult</t>
+  </si>
+  <si>
+    <t>Total New Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewFChild</t>
+  </si>
+  <si>
+    <t>Total New Female Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Female Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewMChild</t>
+  </si>
+  <si>
+    <t>Total New Male Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Male Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.allChildren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Children </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;All Children </t>
+  </si>
+  <si>
+    <t>statistics.allAdults</t>
+  </si>
+  <si>
+    <t>All Adults</t>
+  </si>
+  <si>
+    <t>&amp;All Adults</t>
   </si>
 </sst>
 </file>
@@ -15139,19 +15256,149 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1">
+      <c r="A693" s="36" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B693" s="24" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C693" s="24" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="694" ht="15.75" customHeight="1">
+      <c r="A694" s="23" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B694" s="24" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C694" s="24" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="695" ht="15.75" customHeight="1">
+      <c r="A695" s="23" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B695" s="24" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C695" s="24" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="696" ht="15.75" customHeight="1">
+      <c r="A696" s="23" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B696" s="24" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C696" s="24" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="697" ht="15.75" customHeight="1">
+      <c r="A697" s="23" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B697" s="24" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C697" s="24" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="698" ht="15.75" customHeight="1">
+      <c r="A698" s="23" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B698" s="24" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C698" s="24" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="699" ht="15.75" customHeight="1">
+      <c r="A699" s="23" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B699" s="24" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C699" s="24" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="700" ht="15.75" customHeight="1">
+      <c r="A700" s="23" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B700" s="24" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C700" s="24" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="701" ht="15.75" customHeight="1">
+      <c r="A701" s="23" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B701" s="24" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C701" s="24" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="702" ht="15.75" customHeight="1">
+      <c r="A702" s="23" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B702" s="24" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C702" s="24" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="703" ht="15.75" customHeight="1">
+      <c r="A703" s="23" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B703" s="24" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C703" s="24" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="704" ht="15.75" customHeight="1">
+      <c r="A704" s="23" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B704" s="24" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C704" s="24" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="705" ht="15.75" customHeight="1">
+      <c r="A705" s="23" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B705" s="24" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C705" s="24" t="s">
+        <v>1961</v>
+      </c>
+    </row>
     <row r="706" ht="15.75" customHeight="1"/>
     <row r="707" ht="15.75" customHeight="1"/>
     <row r="708" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
finished base refactoring for stats components
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="1974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="2028">
   <si>
     <t>Key</t>
   </si>
@@ -5945,6 +5945,168 @@
   </si>
   <si>
     <t xml:space="preserve">&amp;Filter by Demographic </t>
+  </si>
+  <si>
+    <t>statistics.femaleChild</t>
+  </si>
+  <si>
+    <t>Female Child</t>
+  </si>
+  <si>
+    <t>&amp;Female Child</t>
+  </si>
+  <si>
+    <t>statistics.maleChild</t>
+  </si>
+  <si>
+    <t>Male Child</t>
+  </si>
+  <si>
+    <t>&amp;Male Child</t>
+  </si>
+  <si>
+    <t>statistics.femaleAdult</t>
+  </si>
+  <si>
+    <t>Female Adult</t>
+  </si>
+  <si>
+    <t>&amp;Female Adult</t>
+  </si>
+  <si>
+    <t>statistics.maleAdult</t>
+  </si>
+  <si>
+    <t>Male Adult</t>
+  </si>
+  <si>
+    <t>&amp;Male Adult</t>
+  </si>
+  <si>
+    <t>statistics.totalFChild</t>
+  </si>
+  <si>
+    <t>Total Female Children:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Children:</t>
+  </si>
+  <si>
+    <t>statistics.totalMChild</t>
+  </si>
+  <si>
+    <t>Total Male Children:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Children:</t>
+  </si>
+  <si>
+    <t>statistics.totalFAdult</t>
+  </si>
+  <si>
+    <t>Total Female Adults:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Adults:</t>
+  </si>
+  <si>
+    <t>statistics.totalMAdult</t>
+  </si>
+  <si>
+    <t>Total Male Adults:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Adults:</t>
+  </si>
+  <si>
+    <t>statistics.totalFChildFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Female Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalMChildFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Male Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalFAdultFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Female Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalMAdultFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Male Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.selectAtLeastOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select at least one Gender and Age option </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Select at least one Gender and Age option </t>
+  </si>
+  <si>
+    <t>statistics.warning</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>&amp;Warning</t>
+  </si>
+  <si>
+    <t>statistics.totalDisFChild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Female Children With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Female Children With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisMChild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Male Chidlren With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Male Chidlren With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisFAdult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Female Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Female Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisMAdult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Male Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Male Adults With Disabilities: </t>
   </si>
 </sst>
 </file>
@@ -15479,24 +15641,204 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1">
+      <c r="A710" s="23" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B710" s="24" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C710" s="24" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="711" ht="15.75" customHeight="1">
+      <c r="A711" s="23" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B711" s="24" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C711" s="24" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="712" ht="15.75" customHeight="1">
+      <c r="A712" s="23" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B712" s="24" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C712" s="24" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="713" ht="15.75" customHeight="1">
+      <c r="A713" s="23" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B713" s="24" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C713" s="24" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="714" ht="15.75" customHeight="1">
+      <c r="A714" s="23" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B714" s="24" t="s">
+        <v>1987</v>
+      </c>
+      <c r="C714" s="24" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="715" ht="15.75" customHeight="1">
+      <c r="A715" s="23" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B715" s="24" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C715" s="24" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="716" ht="15.75" customHeight="1">
+      <c r="A716" s="23" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B716" s="24" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C716" s="24" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="717" ht="15.75" customHeight="1">
+      <c r="A717" s="23" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B717" s="24" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C717" s="24" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="718" ht="15.75" customHeight="1">
+      <c r="A718" s="23" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B718" s="24" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C718" s="24" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="719" ht="15.75" customHeight="1">
+      <c r="A719" s="23" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B719" s="24" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C719" s="24" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="720" ht="15.75" customHeight="1">
+      <c r="A720" s="23" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B720" s="24" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C720" s="24" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="721" ht="15.75" customHeight="1">
+      <c r="A721" s="23" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B721" s="24" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C721" s="24" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="722" ht="15.75" customHeight="1">
+      <c r="A722" s="23" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B722" s="24" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C722" s="24" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="723" ht="15.75" customHeight="1">
+      <c r="A723" s="23" t="s">
+        <v>2013</v>
+      </c>
+      <c r="B723" s="24" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C723" s="24" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="724" ht="15.75" customHeight="1">
+      <c r="A724" s="23" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B724" s="24" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C724" s="24" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="725" ht="15.75" customHeight="1">
+      <c r="A725" s="23" t="s">
+        <v>2019</v>
+      </c>
+      <c r="B725" s="24" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C725" s="24" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="726" ht="15.75" customHeight="1">
+      <c r="A726" s="23" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B726" s="24" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C726" s="24" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="727" ht="15.75" customHeight="1">
+      <c r="A727" s="23" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B727" s="24" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C727" s="24" t="s">
+        <v>2027</v>
+      </c>
+    </row>
     <row r="728" ht="15.75" customHeight="1"/>
     <row r="729" ht="15.75" customHeight="1"/>
     <row r="730" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added translations for the new client field
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="2037">
   <si>
     <t>Key</t>
   </si>
@@ -5801,13 +5801,346 @@
   </si>
   <si>
     <t>&amp;Hover over the details to see more information about each referral.</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpFAdult</t>
+  </si>
+  <si>
+    <t>Total Followed Up Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpMAdult</t>
+  </si>
+  <si>
+    <t>Total Followed Up Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpFChild</t>
+  </si>
+  <si>
+    <t>Total Followed Up Female Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Female Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalFollowedUpMChild</t>
+  </si>
+  <si>
+    <t>Total Followed Up Male Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total Followed Up Male Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.followUpVisits</t>
+  </si>
+  <si>
+    <t>Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.newClients</t>
+  </si>
+  <si>
+    <t>New Clients:</t>
+  </si>
+  <si>
+    <t>&amp;New Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewFAdult</t>
+  </si>
+  <si>
+    <t>Total New Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Female Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewMAdult</t>
+  </si>
+  <si>
+    <t>Total New Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Male Adult Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewFChild</t>
+  </si>
+  <si>
+    <t>Total New Female Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Female Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.totalNewMChild</t>
+  </si>
+  <si>
+    <t>Total New Male Child Clients:</t>
+  </si>
+  <si>
+    <t>&amp;Total New Male Child Clients:</t>
+  </si>
+  <si>
+    <t>statistics.allChildren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Children </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;All Children </t>
+  </si>
+  <si>
+    <t>statistics.allAdults</t>
+  </si>
+  <si>
+    <t>All Adults</t>
+  </si>
+  <si>
+    <t>&amp;All Adults</t>
+  </si>
+  <si>
+    <t>statistics.adult</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>&amp;Adult</t>
+  </si>
+  <si>
+    <t>statistics.child</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>&amp;Child</t>
+  </si>
+  <si>
+    <t>statistics.age</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>&amp;Age</t>
+  </si>
+  <si>
+    <t>statistics.filterByDemographic</t>
+  </si>
+  <si>
+    <t>Filter by Demographic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Filter by Demographic </t>
+  </si>
+  <si>
+    <t>statistics.femaleChild</t>
+  </si>
+  <si>
+    <t>Female Child</t>
+  </si>
+  <si>
+    <t>&amp;Female Child</t>
+  </si>
+  <si>
+    <t>statistics.maleChild</t>
+  </si>
+  <si>
+    <t>Male Child</t>
+  </si>
+  <si>
+    <t>&amp;Male Child</t>
+  </si>
+  <si>
+    <t>statistics.femaleAdult</t>
+  </si>
+  <si>
+    <t>Female Adult</t>
+  </si>
+  <si>
+    <t>&amp;Female Adult</t>
+  </si>
+  <si>
+    <t>statistics.maleAdult</t>
+  </si>
+  <si>
+    <t>Male Adult</t>
+  </si>
+  <si>
+    <t>&amp;Male Adult</t>
+  </si>
+  <si>
+    <t>statistics.totalFChild</t>
+  </si>
+  <si>
+    <t>Total Female Children:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Children:</t>
+  </si>
+  <si>
+    <t>statistics.totalMChild</t>
+  </si>
+  <si>
+    <t>Total Male Children:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Children:</t>
+  </si>
+  <si>
+    <t>statistics.totalFAdult</t>
+  </si>
+  <si>
+    <t>Total Female Adults:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Adults:</t>
+  </si>
+  <si>
+    <t>statistics.totalMAdult</t>
+  </si>
+  <si>
+    <t>Total Male Adults:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Adults:</t>
+  </si>
+  <si>
+    <t>statistics.totalFChildFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Female Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalMChildFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Male Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Children Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalFAdultFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Female Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Female Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.totalMAdultFollowUpVisits</t>
+  </si>
+  <si>
+    <t>Total Male Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>&amp;Total Male Adult Follow Up Visits:</t>
+  </si>
+  <si>
+    <t>statistics.selectAtLeastOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select at least one Gender and Age option </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Select at least one Gender and Age option </t>
+  </si>
+  <si>
+    <t>statistics.warning</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>&amp;Warning</t>
+  </si>
+  <si>
+    <t>statistics.totalDisFChild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Female Children With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Female Children With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisMChild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Male Chidlren With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Male Chidlren With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisFAdult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Female Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Female Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t>statistics.totalDisMAdult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Male Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Total Male Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t>clientFields.hcrType</t>
+  </si>
+  <si>
+    <t>HCR Type</t>
+  </si>
+  <si>
+    <t>&amp;HCR Type</t>
+  </si>
+  <si>
+    <t>clientFields.hostCommunity</t>
+  </si>
+  <si>
+    <t>Host Community</t>
+  </si>
+  <si>
+    <t>&amp;Host Community</t>
+  </si>
+  <si>
+    <t>clientFields.refugee</t>
+  </si>
+  <si>
+    <t>Refugee</t>
+  </si>
+  <si>
+    <t>&amp;Refugee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -5851,8 +6184,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5883,6 +6221,12 @@
         <bgColor rgb="FFF6B26B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -5896,7 +6240,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5985,6 +6329,9 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15159,44 +15506,416 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1">
+      <c r="A694" s="23" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B694" s="24" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C694" s="24" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="695" ht="15.75" customHeight="1">
+      <c r="A695" s="23" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B695" s="24" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C695" s="24" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="696" ht="15.75" customHeight="1">
+      <c r="A696" s="23" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B696" s="24" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C696" s="24" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="697" ht="15.75" customHeight="1">
+      <c r="A697" s="23" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B697" s="24" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C697" s="24" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="698" ht="15.75" customHeight="1">
+      <c r="A698" s="23" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B698" s="24" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C698" s="24" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="699" ht="15.75" customHeight="1">
+      <c r="A699" s="23" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B699" s="24" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C699" s="24" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="700" ht="15.75" customHeight="1">
+      <c r="A700" s="23" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B700" s="24" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C700" s="24" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="701" ht="15.75" customHeight="1">
+      <c r="A701" s="23" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B701" s="24" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C701" s="24" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="702" ht="15.75" customHeight="1">
+      <c r="A702" s="23" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B702" s="24" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C702" s="24" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="703" ht="15.75" customHeight="1">
+      <c r="A703" s="23" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B703" s="24" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C703" s="24" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="704" ht="15.75" customHeight="1">
+      <c r="A704" s="23" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B704" s="24" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C704" s="24" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="705" ht="15.75" customHeight="1">
+      <c r="A705" s="23" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B705" s="24" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C705" s="24" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="706" ht="15.75" customHeight="1">
+      <c r="A706" s="23" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B706" s="24" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C706" s="24" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="707" ht="15.75" customHeight="1">
+      <c r="A707" s="23" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B707" s="24" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C707" s="24" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="708" ht="15.75" customHeight="1">
+      <c r="A708" s="23" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B708" s="24" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C708" s="24" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="709" ht="15.75" customHeight="1">
+      <c r="A709" s="23" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B709" s="24" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C709" s="24" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="710" ht="15.75" customHeight="1">
+      <c r="A710" s="23" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B710" s="24" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C710" s="24" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="711" ht="15.75" customHeight="1">
+      <c r="A711" s="23" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B711" s="24" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C711" s="24" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="712" ht="15.75" customHeight="1">
+      <c r="A712" s="23" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B712" s="24" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C712" s="24" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="713" ht="15.75" customHeight="1">
+      <c r="A713" s="23" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B713" s="24" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C713" s="24" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="714" ht="15.75" customHeight="1">
+      <c r="A714" s="23" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B714" s="24" t="s">
+        <v>1987</v>
+      </c>
+      <c r="C714" s="24" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="715" ht="15.75" customHeight="1">
+      <c r="A715" s="23" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B715" s="24" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C715" s="24" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="716" ht="15.75" customHeight="1">
+      <c r="A716" s="23" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B716" s="24" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C716" s="24" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="717" ht="15.75" customHeight="1">
+      <c r="A717" s="23" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B717" s="24" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C717" s="24" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="718" ht="15.75" customHeight="1">
+      <c r="A718" s="23" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B718" s="24" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C718" s="24" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="719" ht="15.75" customHeight="1">
+      <c r="A719" s="23" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B719" s="24" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C719" s="24" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="720" ht="15.75" customHeight="1">
+      <c r="A720" s="23" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B720" s="24" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C720" s="24" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="721" ht="15.75" customHeight="1">
+      <c r="A721" s="23" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B721" s="24" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C721" s="24" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="722" ht="15.75" customHeight="1">
+      <c r="A722" s="23" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B722" s="24" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C722" s="24" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="723" ht="15.75" customHeight="1">
+      <c r="A723" s="23" t="s">
+        <v>2013</v>
+      </c>
+      <c r="B723" s="24" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C723" s="24" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="724" ht="15.75" customHeight="1">
+      <c r="A724" s="23" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B724" s="24" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C724" s="24" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="725" ht="15.75" customHeight="1">
+      <c r="A725" s="23" t="s">
+        <v>2019</v>
+      </c>
+      <c r="B725" s="24" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C725" s="24" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="726" ht="15.75" customHeight="1">
+      <c r="A726" s="23" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B726" s="24" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C726" s="24" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="727" ht="15.75" customHeight="1">
+      <c r="A727" s="23" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B727" s="24" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C727" s="24" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="728" ht="15.75" customHeight="1">
+      <c r="A728" s="23" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B728" s="24" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C728" s="24" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="729" ht="15.75" customHeight="1">
+      <c r="A729" s="23" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B729" s="24" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C729" s="24" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="730" ht="15.75" customHeight="1">
+      <c r="A730" s="23" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B730" s="24" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C730" s="24" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="731" ht="15.75" customHeight="1">
+      <c r="A731" s="37"/>
+    </row>
     <row r="732" ht="15.75" customHeight="1"/>
     <row r="733" ht="15.75" customHeight="1"/>
     <row r="734" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updated web stats translations
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="2028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="2043">
   <si>
     <t>Key</t>
   </si>
@@ -6107,13 +6107,58 @@
   </si>
   <si>
     <t xml:space="preserve">&amp;Total Male Adults With Disabilities: </t>
+  </si>
+  <si>
+    <t>clientFields.hcrType</t>
+  </si>
+  <si>
+    <t>HCR Type</t>
+  </si>
+  <si>
+    <t>&amp;HCR Type</t>
+  </si>
+  <si>
+    <t>clientFields.hostCommunity</t>
+  </si>
+  <si>
+    <t>Host Community</t>
+  </si>
+  <si>
+    <t>&amp;Host Community</t>
+  </si>
+  <si>
+    <t>clientFields.refugee</t>
+  </si>
+  <si>
+    <t>Refugee</t>
+  </si>
+  <si>
+    <t>&amp;Refugee</t>
+  </si>
+  <si>
+    <t>statistics.specificDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Specific Date </t>
+  </si>
+  <si>
+    <t>statistics.monthly</t>
+  </si>
+  <si>
+    <t>By Month</t>
+  </si>
+  <si>
+    <t>&amp;By Month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6156,6 +6201,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -6202,7 +6252,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6291,6 +6341,9 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15839,11 +15892,61 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1">
+      <c r="A728" s="23" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B728" s="24" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C728" s="24" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="729" ht="15.75" customHeight="1">
+      <c r="A729" s="23" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B729" s="24" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C729" s="24" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="730" ht="15.75" customHeight="1">
+      <c r="A730" s="23" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B730" s="24" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C730" s="24" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="731" ht="15.75" customHeight="1">
+      <c r="A731" s="37" t="s">
+        <v>2037</v>
+      </c>
+      <c r="B731" s="24" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C731" s="24" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="732" ht="15.75" customHeight="1">
+      <c r="A732" s="23" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B732" s="24" t="s">
+        <v>2041</v>
+      </c>
+      <c r="C732" s="24" t="s">
+        <v>2042</v>
+      </c>
+    </row>
     <row r="733" ht="15.75" customHeight="1"/>
     <row r="734" ht="15.75" customHeight="1"/>
     <row r="735" ht="15.75" customHeight="1"/>
@@ -16103,7 +16206,7 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A990">
+  <conditionalFormatting sqref="A1:A990 B738">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF (A:A, A1)&gt;1</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix: remove i18next::pluralResolver warn
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -1374,10 +1374,10 @@
     <t>alert.messageAlert</t>
   </si>
   <si>
-    <t>You have {{count}} new messages in your inbox.</t>
-  </si>
-  <si>
-    <t>Do a nyu' {{count}} longiyo lo luduk kulo konuk yi su'de ni</t>
+    <t>You have {{numMessages}} new messages in your inbox.</t>
+  </si>
+  <si>
+    <t>Do a nyu' {{numMessages}} longiyo lo luduk kulo konuk yi su'de ni</t>
   </si>
   <si>
     <t>alert.unauthorizedArchive</t>
@@ -8648,7 +8648,7 @@
       <c r="A152" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="B152" s="8" t="s">
+      <c r="B152" s="11" t="s">
         <v>452</v>
       </c>
       <c r="C152" s="11" t="s">

</xml_diff>

<commit_message>
fix: update translations file and use goal fields instead of placeholders
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexe\source\415-HHA-CBR\common\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75C854-0FAF-4B74-A35D-AF5D80BCF803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F8BE24-CBEC-4B8F-8168-D3539C9F5A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="1977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1980">
   <si>
     <t>Key</t>
   </si>
@@ -5974,6 +5974,15 @@
   </si>
   <si>
     <t>All Adults</t>
+  </si>
+  <si>
+    <t>risks.goalAchieved</t>
+  </si>
+  <si>
+    <t>risks.goalInProgress</t>
+  </si>
+  <si>
+    <t>risks.goalCancelled</t>
   </si>
 </sst>
 </file>
@@ -6334,10 +6343,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1005"/>
+  <dimension ref="A1:E1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A640" workbookViewId="0">
-      <selection activeCell="B647" sqref="B647"/>
+    <sheetView tabSelected="1" topLeftCell="A677" workbookViewId="0">
+      <selection activeCell="B689" sqref="B689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15004,7 +15013,7 @@
         <v>1854</v>
       </c>
       <c r="C670" s="14" t="str">
-        <f t="shared" ref="C670:C702" si="0">CONCATENATE("&amp;", B670)</f>
+        <f t="shared" ref="C670:C705" si="0">CONCATENATE("&amp;", B670)</f>
         <v>&amp;Improve connection with community</v>
       </c>
     </row>
@@ -15393,96 +15402,129 @@
       </c>
     </row>
     <row r="703" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A703" s="21" t="s">
+      <c r="A703" s="18" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B703" s="14" t="s">
+        <v>1879</v>
+      </c>
+      <c r="C703" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp;Achieved</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A704" s="18" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B704" s="14" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C704" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp;In progress</v>
+      </c>
+    </row>
+    <row r="705" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A705" s="18" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B705" s="14" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C705" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp;Cancelled</v>
+      </c>
+    </row>
+    <row r="706" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A706" s="21" t="s">
         <v>1902</v>
       </c>
-      <c r="B703" s="20" t="s">
+      <c r="B706" s="20" t="s">
         <v>1903</v>
       </c>
-      <c r="C703" s="20" t="s">
+      <c r="C706" s="20" t="s">
         <v>1904</v>
-      </c>
-    </row>
-    <row r="704" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A704" s="21" t="s">
-        <v>1905</v>
-      </c>
-      <c r="B704" s="20" t="s">
-        <v>1906</v>
-      </c>
-      <c r="C704" s="20" t="s">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="705" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A705" s="21" t="s">
-        <v>1908</v>
-      </c>
-      <c r="B705" s="20" t="s">
-        <v>1909</v>
-      </c>
-      <c r="C705" s="20" t="s">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="706" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A706" s="21" t="s">
-        <v>1911</v>
-      </c>
-      <c r="B706" s="20" t="s">
-        <v>1912</v>
-      </c>
-      <c r="C706" s="20" t="s">
-        <v>1913</v>
       </c>
     </row>
     <row r="707" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A707" s="21" t="s">
-        <v>1914</v>
+        <v>1905</v>
       </c>
       <c r="B707" s="20" t="s">
-        <v>1915</v>
+        <v>1906</v>
       </c>
       <c r="C707" s="20" t="s">
-        <v>1916</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="708" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A708" s="21" t="s">
-        <v>1917</v>
-      </c>
-      <c r="B708" s="14" t="s">
-        <v>1918</v>
-      </c>
-      <c r="C708" s="14" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="709" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1908</v>
+      </c>
+      <c r="B708" s="20" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C708" s="20" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="709" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A709" s="21" t="s">
-        <v>1920</v>
-      </c>
-      <c r="B709" s="14" t="s">
-        <v>1921</v>
-      </c>
-      <c r="C709" s="14" t="s">
-        <v>1922</v>
+        <v>1911</v>
+      </c>
+      <c r="B709" s="20" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C709" s="20" t="s">
+        <v>1913</v>
       </c>
     </row>
     <row r="710" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A710" s="21" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B710" s="20" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C710" s="20" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="711" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A711" s="21" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B711" s="14" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C711" s="14" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="712" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A712" s="21" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B712" s="14" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C712" s="14" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A713" s="21" t="s">
         <v>1923</v>
       </c>
-      <c r="B710" s="14" t="s">
+      <c r="B713" s="14" t="s">
         <v>1924</v>
       </c>
-      <c r="C710" s="14" t="s">
+      <c r="C713" s="14" t="s">
         <v>1925</v>
       </c>
     </row>
-    <row r="711" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="714" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="715" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="716" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15775,6 +15817,9 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
678 fix trasnaltions and update translateGoalStatusSummary helper
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="2137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="2152">
   <si>
     <t>Key</t>
   </si>
@@ -6434,6 +6434,51 @@
   </si>
   <si>
     <t>&amp;Client's Mental Health Goal Requirements</t>
+  </si>
+  <si>
+    <t>goals.healthSet</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;Health&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>&amp;&lt;1&gt;Health&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>goals.educationSet</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;Education&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>&amp;&lt;1&gt;Education&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>goals.socialSet</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;Social&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>&amp;&lt;1&gt;Social&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>goals.nutritionSet</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;Nutrition&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>&amp;&lt;1&gt;Nutrition&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>goals.mentalSet</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;Mental Health&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>&amp;&lt;1&gt;Mental Health&lt;/1&gt; goal status set to</t>
   </si>
 </sst>
 </file>
@@ -6495,7 +6540,7 @@
       <name val="&quot;Noto Mono&quot;"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6544,6 +6589,12 @@
         <bgColor rgb="FFF6B26B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4A7D6"/>
+        <bgColor rgb="FFB4A7D6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -6551,7 +6602,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6673,6 +6724,9 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -16630,11 +16684,61 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1">
+      <c r="A765" s="49" t="s">
+        <v>2137</v>
+      </c>
+      <c r="B765" s="47" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C765" s="47" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="766" ht="15.75" customHeight="1">
+      <c r="A766" s="49" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B766" s="47" t="s">
+        <v>2141</v>
+      </c>
+      <c r="C766" s="47" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="767" ht="15.75" customHeight="1">
+      <c r="A767" s="49" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B767" s="47" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C767" s="47" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="768" ht="15.75" customHeight="1">
+      <c r="A768" s="49" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B768" s="47" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C768" s="47" t="s">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="769" ht="15.75" customHeight="1">
+      <c r="A769" s="49" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B769" s="47" t="s">
+        <v>2150</v>
+      </c>
+      <c r="C769" s="47" t="s">
+        <v>2151</v>
+      </c>
+    </row>
     <row r="770" ht="15.75" customHeight="1"/>
     <row r="771" ht="15.75" customHeight="1"/>
     <row r="772" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: add confirmation dialog to back button
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="H1qyQ/Z23RlVQBZ0QoeK0uXawsEM5dJo9S4H91T6u/Y="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="QH1aKaMXwk8uW8hJGBOI0dPvHLxJt76JORECZvXqFrE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="2152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="2155">
   <si>
     <t>Key</t>
   </si>
@@ -30,7 +30,9 @@
     <t>_COPIED_WARNING</t>
   </si>
   <si>
-    <t>DO NOT EDIT THIS FILE; it is generated by the 'update-translations' script</t>
+    <t>DO NOT EDIT THIS FILE; it is generated by the 'update-translations' script
+Only edit file "Translations_CBR_main.xlsx" on the Google Drive
+Do not edit the .json files directly.</t>
   </si>
   <si>
     <t>login.login</t>
@@ -6479,6 +6481,15 @@
   </si>
   <si>
     <t>&amp;&lt;1&gt;Mental Health&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>general.goBackWarning</t>
+  </si>
+  <si>
+    <t>You may have unsaved changes. Are you sure you want to go back?</t>
+  </si>
+  <si>
+    <t>&amp;You may have unsaved changes. Are you sure you want to go back?</t>
   </si>
 </sst>
 </file>
@@ -6540,7 +6551,7 @@
       <name val="&quot;Noto Mono&quot;"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6591,6 +6602,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
         <bgColor rgb="FFB4A7D6"/>
       </patternFill>
@@ -6602,7 +6619,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6725,6 +6742,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -6975,7 +6998,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -16564,7 +16587,7 @@
       </c>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="A754" s="40" t="s">
+      <c r="A754" s="49" t="s">
         <v>2104</v>
       </c>
       <c r="B754" s="16" t="s">
@@ -16685,7 +16708,7 @@
       </c>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="A765" s="49" t="s">
+      <c r="A765" s="50" t="s">
         <v>2137</v>
       </c>
       <c r="B765" s="47" t="s">
@@ -16696,7 +16719,7 @@
       </c>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="A766" s="49" t="s">
+      <c r="A766" s="50" t="s">
         <v>2140</v>
       </c>
       <c r="B766" s="47" t="s">
@@ -16707,7 +16730,7 @@
       </c>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="A767" s="49" t="s">
+      <c r="A767" s="50" t="s">
         <v>2143</v>
       </c>
       <c r="B767" s="47" t="s">
@@ -16718,7 +16741,7 @@
       </c>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="A768" s="49" t="s">
+      <c r="A768" s="50" t="s">
         <v>2146</v>
       </c>
       <c r="B768" s="47" t="s">
@@ -16729,7 +16752,7 @@
       </c>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="A769" s="49" t="s">
+      <c r="A769" s="50" t="s">
         <v>2149</v>
       </c>
       <c r="B769" s="47" t="s">
@@ -16739,7 +16762,19 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1">
+      <c r="A770" s="51" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B770" s="11" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C770" s="11" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D770" s="4"/>
+      <c r="E770" s="4"/>
+    </row>
     <row r="771" ht="15.75" customHeight="1"/>
     <row r="772" ht="15.75" customHeight="1"/>
     <row r="773" ht="15.75" customHeight="1"/>
@@ -16905,8 +16940,9 @@
     <row r="933" ht="15.75" customHeight="1"/>
     <row r="934" ht="15.75" customHeight="1"/>
     <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A935 B572">
+  <conditionalFormatting sqref="A1:A936 B572">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF (A:A, A1)&gt;1</formula>
     </cfRule>

</xml_diff>

<commit_message>
feat: update translations and change dropdown text to use i18
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="H1qyQ/Z23RlVQBZ0QoeK0uXawsEM5dJo9S4H91T6u/Y="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="QH1aKaMXwk8uW8hJGBOI0dPvHLxJt76JORECZvXqFrE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="2152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="2286">
   <si>
     <t>Key</t>
   </si>
@@ -30,7 +30,9 @@
     <t>_COPIED_WARNING</t>
   </si>
   <si>
-    <t>DO NOT EDIT THIS FILE; it is generated by the 'update-translations' script</t>
+    <t>DO NOT EDIT THIS FILE; it is generated by the 'update-translations' script
+Only edit file "Translations_CBR_main.xlsx" on the Google Drive
+Do not edit the .json files directly.</t>
   </si>
   <si>
     <t>login.login</t>
@@ -6479,6 +6481,408 @@
   </si>
   <si>
     <t>&amp;&lt;1&gt;Mental Health&lt;/1&gt; goal status set to</t>
+  </si>
+  <si>
+    <t>general.goBackWarning</t>
+  </si>
+  <si>
+    <t>You may have unsaved changes. Are you sure you want to go back?</t>
+  </si>
+  <si>
+    <t>&amp;You may have unsaved changes. Are you sure you want to go back?</t>
+  </si>
+  <si>
+    <t>cancellation.dead</t>
+  </si>
+  <si>
+    <t>Patient has died</t>
+  </si>
+  <si>
+    <t>&amp;Patient has died</t>
+  </si>
+  <si>
+    <t>cancellation.moved</t>
+  </si>
+  <si>
+    <t>Patient has moved away</t>
+  </si>
+  <si>
+    <t>&amp;Patient has moved away</t>
+  </si>
+  <si>
+    <t>cancellation.circumstances</t>
+  </si>
+  <si>
+    <t>Patient's circumstances have changed</t>
+  </si>
+  <si>
+    <t>&amp;Patient's circumstances have changed</t>
+  </si>
+  <si>
+    <t>cancellation.abandoned</t>
+  </si>
+  <si>
+    <t>Patient has abandoned this goal</t>
+  </si>
+  <si>
+    <t>&amp;Patient has abandoned this goal</t>
+  </si>
+  <si>
+    <t>cancellation.unwilling</t>
+  </si>
+  <si>
+    <t>Patient is no longer willing to work with us</t>
+  </si>
+  <si>
+    <t>&amp;Patient is no longer willing to work with us</t>
+  </si>
+  <si>
+    <t>risk.healthRequirementMalaria</t>
+  </si>
+  <si>
+    <t>Malaria treatment</t>
+  </si>
+  <si>
+    <t>&amp;Malaria treatment</t>
+  </si>
+  <si>
+    <t>risk.healthRequirementMedical</t>
+  </si>
+  <si>
+    <t>Medical assistance</t>
+  </si>
+  <si>
+    <t>&amp;Medical assistance</t>
+  </si>
+  <si>
+    <t>risk.healthRequirementWound</t>
+  </si>
+  <si>
+    <t>Wound care for pressure sores</t>
+  </si>
+  <si>
+    <t>&amp;Wound care for pressure sores</t>
+  </si>
+  <si>
+    <t>risk.healthRequirementMobility</t>
+  </si>
+  <si>
+    <t>Mobility device - crutches</t>
+  </si>
+  <si>
+    <t>wheelchair etc</t>
+  </si>
+  <si>
+    <t>risk.healthRequirementPhysiotherapy</t>
+  </si>
+  <si>
+    <t>&amp;Physiotherapy</t>
+  </si>
+  <si>
+    <t>risk.healthGoalMedical</t>
+  </si>
+  <si>
+    <t>Medical treatment provided</t>
+  </si>
+  <si>
+    <t>&amp;Medical treatment provided</t>
+  </si>
+  <si>
+    <t>risk.healthGoalSores</t>
+  </si>
+  <si>
+    <t>Sores managed/healed</t>
+  </si>
+  <si>
+    <t>&amp;Sores managed/healed</t>
+  </si>
+  <si>
+    <t>risk.healthGoalMobility</t>
+  </si>
+  <si>
+    <t>Mobility device provided</t>
+  </si>
+  <si>
+    <t>&amp;Mobility device provided</t>
+  </si>
+  <si>
+    <t>risk.healthGoalPain</t>
+  </si>
+  <si>
+    <t>Pain managed</t>
+  </si>
+  <si>
+    <t>&amp;Pain managed</t>
+  </si>
+  <si>
+    <t>risk.socialRequirementContact</t>
+  </si>
+  <si>
+    <t>Contact with community</t>
+  </si>
+  <si>
+    <t>&amp;Contact with community</t>
+  </si>
+  <si>
+    <t>risk.socialRequirementInclusion</t>
+  </si>
+  <si>
+    <t>Inclusion in family</t>
+  </si>
+  <si>
+    <t>&amp;Inclusion in family</t>
+  </si>
+  <si>
+    <t>risk.socialRequirementTraining</t>
+  </si>
+  <si>
+    <t>Training for family members</t>
+  </si>
+  <si>
+    <t>&amp;Training for family members</t>
+  </si>
+  <si>
+    <t>risk.socialGoalCommunity</t>
+  </si>
+  <si>
+    <t>Take part in a community event</t>
+  </si>
+  <si>
+    <t>&amp;Take part in a community event</t>
+  </si>
+  <si>
+    <t>risk.socialGoalInclusion</t>
+  </si>
+  <si>
+    <t>Inclusion in family time</t>
+  </si>
+  <si>
+    <t>&amp;Inclusion in family time</t>
+  </si>
+  <si>
+    <t>risk.nutritionRequirementDiabetic</t>
+  </si>
+  <si>
+    <t>Special dietary need - diabetic</t>
+  </si>
+  <si>
+    <t>&amp;Special dietary need - diabetic</t>
+  </si>
+  <si>
+    <t>risk.nutritionRequirementAllergies</t>
+  </si>
+  <si>
+    <t>Special dietary need - allergies</t>
+  </si>
+  <si>
+    <t>&amp;Special dietary need - allergies</t>
+  </si>
+  <si>
+    <t>risk.nutritionRequirementMalnutrition</t>
+  </si>
+  <si>
+    <t>Special dietary need - malnutrition</t>
+  </si>
+  <si>
+    <t>&amp;Special dietary need - malnutrition</t>
+  </si>
+  <si>
+    <t>risk.nutritionRequirementTraining</t>
+  </si>
+  <si>
+    <t>Nutrition training</t>
+  </si>
+  <si>
+    <t>&amp;Nutrition training</t>
+  </si>
+  <si>
+    <t>risk.nutritionRequirementAgricultural</t>
+  </si>
+  <si>
+    <t>Inclusion in Agricultural project</t>
+  </si>
+  <si>
+    <t>&amp;Inclusion in Agricultural project</t>
+  </si>
+  <si>
+    <t>risk.nutritionGoalManageDiet</t>
+  </si>
+  <si>
+    <t>Manage diet to meet needs</t>
+  </si>
+  <si>
+    <t>&amp;Manage diet to meet needs</t>
+  </si>
+  <si>
+    <t>risk.nutritionGoalSustainable</t>
+  </si>
+  <si>
+    <t>Sustainable food source</t>
+  </si>
+  <si>
+    <t>&amp;Sustainable food source</t>
+  </si>
+  <si>
+    <t>risk.educationRequirementSchool</t>
+  </si>
+  <si>
+    <t>Attend school</t>
+  </si>
+  <si>
+    <t>&amp;Attend school</t>
+  </si>
+  <si>
+    <t>risk.educationRequirementVocational</t>
+  </si>
+  <si>
+    <t>Vocational training</t>
+  </si>
+  <si>
+    <t>&amp;Vocational training</t>
+  </si>
+  <si>
+    <t>risk.educationRequirementFamily</t>
+  </si>
+  <si>
+    <t>Training for family - learning through play</t>
+  </si>
+  <si>
+    <t>&amp;Training for family - learning through play</t>
+  </si>
+  <si>
+    <t>risk.educationGoalEducation</t>
+  </si>
+  <si>
+    <t>Have an education</t>
+  </si>
+  <si>
+    <t>&amp;Have an education</t>
+  </si>
+  <si>
+    <t>risk.educationGoalIncome</t>
+  </si>
+  <si>
+    <t>Sustainable source of income</t>
+  </si>
+  <si>
+    <t>&amp;Sustainable source of income</t>
+  </si>
+  <si>
+    <t>risk.educationGoalChild</t>
+  </si>
+  <si>
+    <t>Child ready to start school</t>
+  </si>
+  <si>
+    <t>&amp;Child ready to start school</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementMedical</t>
+  </si>
+  <si>
+    <t>Needs medical attention</t>
+  </si>
+  <si>
+    <t>&amp;Needs medical attention</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementFamily</t>
+  </si>
+  <si>
+    <t>Promote understanding in the family</t>
+  </si>
+  <si>
+    <t>&amp;Promote understanding in the family</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementCommunity</t>
+  </si>
+  <si>
+    <t>Promote understanding in the community</t>
+  </si>
+  <si>
+    <t>&amp;Promote understanding in the community</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementRefer</t>
+  </si>
+  <si>
+    <t>Refer to mental health agencies</t>
+  </si>
+  <si>
+    <t>&amp;Refer to mental health agencies</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementCounsellingStressTrauma</t>
+  </si>
+  <si>
+    <t>Advice and counselling - stress and trauma</t>
+  </si>
+  <si>
+    <t>&amp;Advice and counselling - stress and trauma</t>
+  </si>
+  <si>
+    <t>risk.mentalRequirementCounsellingOther</t>
+  </si>
+  <si>
+    <t>Advice and counselling - other</t>
+  </si>
+  <si>
+    <t>&amp;Advice and counselling - other</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalFamily</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalCommunity</t>
+  </si>
+  <si>
+    <t>Inclusion in community</t>
+  </si>
+  <si>
+    <t>&amp;Inclusion in community</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalMedical</t>
+  </si>
+  <si>
+    <t>Medical assistance provided</t>
+  </si>
+  <si>
+    <t>&amp;Medical assistance provided</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalAgency</t>
+  </si>
+  <si>
+    <t>Seen by mental health agency</t>
+  </si>
+  <si>
+    <t>&amp;Seen by mental health agency</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalImprovement</t>
+  </si>
+  <si>
+    <t>Improvement in mental health</t>
+  </si>
+  <si>
+    <t>&amp;Improvement in mental health</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalReduction</t>
+  </si>
+  <si>
+    <t>Reduction of stress and trauma</t>
+  </si>
+  <si>
+    <t>&amp;Reduction of stress and trauma</t>
+  </si>
+  <si>
+    <t>risk.mentalGoalImprovements</t>
+  </si>
+  <si>
+    <t>&amp;Improvements</t>
   </si>
 </sst>
 </file>
@@ -6540,7 +6944,7 @@
       <name val="&quot;Noto Mono&quot;"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6591,6 +6995,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
         <bgColor rgb="FFB4A7D6"/>
       </patternFill>
@@ -6602,7 +7012,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6725,6 +7135,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -6975,7 +7391,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -16564,7 +16980,7 @@
       </c>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="A754" s="40" t="s">
+      <c r="A754" s="49" t="s">
         <v>2104</v>
       </c>
       <c r="B754" s="16" t="s">
@@ -16685,7 +17101,7 @@
       </c>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="A765" s="49" t="s">
+      <c r="A765" s="50" t="s">
         <v>2137</v>
       </c>
       <c r="B765" s="47" t="s">
@@ -16696,7 +17112,7 @@
       </c>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="A766" s="49" t="s">
+      <c r="A766" s="50" t="s">
         <v>2140</v>
       </c>
       <c r="B766" s="47" t="s">
@@ -16707,7 +17123,7 @@
       </c>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="A767" s="49" t="s">
+      <c r="A767" s="50" t="s">
         <v>2143</v>
       </c>
       <c r="B767" s="47" t="s">
@@ -16718,7 +17134,7 @@
       </c>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="A768" s="49" t="s">
+      <c r="A768" s="50" t="s">
         <v>2146</v>
       </c>
       <c r="B768" s="47" t="s">
@@ -16729,7 +17145,7 @@
       </c>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="A769" s="49" t="s">
+      <c r="A769" s="50" t="s">
         <v>2149</v>
       </c>
       <c r="B769" s="47" t="s">
@@ -16739,52 +17155,514 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1">
+      <c r="A770" s="51" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B770" s="11" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C770" s="11" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D770" s="4"/>
+      <c r="E770" s="4"/>
+    </row>
+    <row r="771" ht="15.75" customHeight="1">
+      <c r="A771" s="40" t="s">
+        <v>2155</v>
+      </c>
+      <c r="B771" s="16" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C771" s="16" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="772" ht="15.75" customHeight="1">
+      <c r="A772" s="40" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B772" s="16" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C772" s="16" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="773" ht="15.75" customHeight="1">
+      <c r="A773" s="40" t="s">
+        <v>2161</v>
+      </c>
+      <c r="B773" s="16" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C773" s="16" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="774" ht="15.75" customHeight="1">
+      <c r="A774" s="40" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B774" s="16" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C774" s="16" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="775" ht="15.75" customHeight="1">
+      <c r="A775" s="40" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B775" s="16" t="s">
+        <v>2168</v>
+      </c>
+      <c r="C775" s="16" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="776" ht="15.75" customHeight="1">
+      <c r="A776" s="40" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B776" s="16" t="s">
+        <v>2171</v>
+      </c>
+      <c r="C776" s="16" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="777" ht="15.75" customHeight="1">
+      <c r="A777" s="40" t="s">
+        <v>2173</v>
+      </c>
+      <c r="B777" s="16" t="s">
+        <v>2174</v>
+      </c>
+      <c r="C777" s="16" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="778" ht="15.75" customHeight="1">
+      <c r="A778" s="40" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B778" s="16" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C778" s="16" t="s">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="779" ht="15.75" customHeight="1">
+      <c r="A779" s="40" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B779" s="16" t="s">
+        <v>2180</v>
+      </c>
+      <c r="C779" s="16" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="780" ht="15.75" customHeight="1">
+      <c r="A780" s="40" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B780" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="C780" s="16" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="781" ht="15.75" customHeight="1">
+      <c r="A781" s="40" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B781" s="16" t="s">
+        <v>2185</v>
+      </c>
+      <c r="C781" s="16" t="s">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="782" ht="15.75" customHeight="1">
+      <c r="A782" s="40" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B782" s="16" t="s">
+        <v>2188</v>
+      </c>
+      <c r="C782" s="16" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="783" ht="15.75" customHeight="1">
+      <c r="A783" s="40" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B783" s="16" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C783" s="16" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="784" ht="15.75" customHeight="1">
+      <c r="A784" s="40" t="s">
+        <v>2193</v>
+      </c>
+      <c r="B784" s="16" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C784" s="16" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="785" ht="15.75" customHeight="1">
+      <c r="A785" s="40" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B785" s="16" t="s">
+        <v>2197</v>
+      </c>
+      <c r="C785" s="16" t="s">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="786" ht="15.75" customHeight="1">
+      <c r="A786" s="40" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B786" s="16" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C786" s="16" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="787" ht="15.75" customHeight="1">
+      <c r="A787" s="40" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B787" s="16" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C787" s="16" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="788" ht="15.75" customHeight="1">
+      <c r="A788" s="40" t="s">
+        <v>2205</v>
+      </c>
+      <c r="B788" s="16" t="s">
+        <v>2206</v>
+      </c>
+      <c r="C788" s="16" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="789" ht="15.75" customHeight="1">
+      <c r="A789" s="40" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B789" s="16" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C789" s="16" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="790" ht="15.75" customHeight="1">
+      <c r="A790" s="40" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B790" s="16" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C790" s="16" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="791" ht="15.75" customHeight="1">
+      <c r="A791" s="40" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B791" s="16" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C791" s="16" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="792" ht="15.75" customHeight="1">
+      <c r="A792" s="40" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B792" s="16" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C792" s="16" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="793" ht="15.75" customHeight="1">
+      <c r="A793" s="40" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B793" s="16" t="s">
+        <v>2221</v>
+      </c>
+      <c r="C793" s="16" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="794" ht="15.75" customHeight="1">
+      <c r="A794" s="40" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B794" s="16" t="s">
+        <v>2224</v>
+      </c>
+      <c r="C794" s="16" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="795" ht="15.75" customHeight="1">
+      <c r="A795" s="40" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B795" s="16" t="s">
+        <v>2227</v>
+      </c>
+      <c r="C795" s="16" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="796" ht="15.75" customHeight="1">
+      <c r="A796" s="40" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B796" s="16" t="s">
+        <v>2230</v>
+      </c>
+      <c r="C796" s="16" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="797" ht="15.75" customHeight="1">
+      <c r="A797" s="40" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B797" s="16" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C797" s="16" t="s">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="798" ht="15.75" customHeight="1">
+      <c r="A798" s="40" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B798" s="16" t="s">
+        <v>2236</v>
+      </c>
+      <c r="C798" s="16" t="s">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="799" ht="15.75" customHeight="1">
+      <c r="A799" s="40" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B799" s="16" t="s">
+        <v>2239</v>
+      </c>
+      <c r="C799" s="16" t="s">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="800" ht="15.75" customHeight="1">
+      <c r="A800" s="40" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B800" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="C800" s="16" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="801" ht="15.75" customHeight="1">
+      <c r="A801" s="40" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B801" s="16" t="s">
+        <v>2245</v>
+      </c>
+      <c r="C801" s="16" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="802" ht="15.75" customHeight="1">
+      <c r="A802" s="40" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B802" s="16" t="s">
+        <v>2248</v>
+      </c>
+      <c r="C802" s="16" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="803" ht="15.75" customHeight="1">
+      <c r="A803" s="40" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B803" s="16" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C803" s="16" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="804" ht="15.75" customHeight="1">
+      <c r="A804" s="40" t="s">
+        <v>2253</v>
+      </c>
+      <c r="B804" s="16" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C804" s="16" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="805" ht="15.75" customHeight="1">
+      <c r="A805" s="40" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B805" s="16" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C805" s="16" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="806" ht="15.75" customHeight="1">
+      <c r="A806" s="40" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B806" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="C806" s="16" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="807" ht="15.75" customHeight="1">
+      <c r="A807" s="40" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B807" s="16" t="s">
+        <v>2263</v>
+      </c>
+      <c r="C807" s="16" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="808" ht="15.75" customHeight="1">
+      <c r="A808" s="40" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B808" s="16" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C808" s="16" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="809" ht="15.75" customHeight="1">
+      <c r="A809" s="40" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B809" s="16" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C809" s="16" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="810" ht="15.75" customHeight="1">
+      <c r="A810" s="40" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B810" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="C810" s="16" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="811" ht="15.75" customHeight="1">
+      <c r="A811" s="40" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B811" s="16" t="s">
+        <v>2273</v>
+      </c>
+      <c r="C811" s="16" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="812" ht="15.75" customHeight="1">
+      <c r="A812" s="40" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B812" s="16" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C812" s="16" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="813" ht="15.75" customHeight="1">
+      <c r="A813" s="40" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B813" s="16" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C813" s="16" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="814" ht="15.75" customHeight="1">
+      <c r="A814" s="40" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B814" s="16" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C814" s="16" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="815" ht="15.75" customHeight="1">
+      <c r="A815" s="40" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B815" s="16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C815" s="16" t="s">
+        <v>2285</v>
+      </c>
+    </row>
     <row r="816" ht="15.75" customHeight="1"/>
     <row r="817" ht="15.75" customHeight="1"/>
     <row r="818" ht="15.75" customHeight="1"/>
@@ -16905,8 +17783,9 @@
     <row r="933" ht="15.75" customHeight="1"/>
     <row r="934" ht="15.75" customHeight="1"/>
     <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A935 B572">
+  <conditionalFormatting sqref="A1:A770 B572 A816:A936">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF (A:A, A1)&gt;1</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix: update translation file formatting
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -6537,7 +6537,7 @@
     <t>&amp;Patient is no longer willing to work with us</t>
   </si>
   <si>
-    <t>risk.healthRequirementMalaria</t>
+    <t>risk.health.requirement.Malaria</t>
   </si>
   <si>
     <t>Malaria treatment</t>
@@ -6546,7 +6546,7 @@
     <t>&amp;Malaria treatment</t>
   </si>
   <si>
-    <t>risk.healthRequirementMedical</t>
+    <t>risk.health.requirement.Medical</t>
   </si>
   <si>
     <t>Medical assistance</t>
@@ -6555,7 +6555,7 @@
     <t>&amp;Medical assistance</t>
   </si>
   <si>
-    <t>risk.healthRequirementWound</t>
+    <t>risk.health.requirement.Wound</t>
   </si>
   <si>
     <t>Wound care for pressure sores</t>
@@ -6564,7 +6564,7 @@
     <t>&amp;Wound care for pressure sores</t>
   </si>
   <si>
-    <t>risk.healthRequirementMobility</t>
+    <t>risk.health.requirement.Mobility</t>
   </si>
   <si>
     <t>Mobility device - crutches</t>
@@ -6573,13 +6573,13 @@
     <t>wheelchair etc</t>
   </si>
   <si>
-    <t>risk.healthRequirementPhysiotherapy</t>
+    <t>risk.health.requirement.Physiotherapy</t>
   </si>
   <si>
     <t>&amp;Physiotherapy</t>
   </si>
   <si>
-    <t>risk.healthGoalMedical</t>
+    <t>risk.health.goal.Medical</t>
   </si>
   <si>
     <t>Medical treatment provided</t>
@@ -6588,7 +6588,7 @@
     <t>&amp;Medical treatment provided</t>
   </si>
   <si>
-    <t>risk.healthGoalSores</t>
+    <t>risk.health.goal.Sores</t>
   </si>
   <si>
     <t>Sores managed/healed</t>
@@ -6597,7 +6597,7 @@
     <t>&amp;Sores managed/healed</t>
   </si>
   <si>
-    <t>risk.healthGoalMobility</t>
+    <t>risk.health.goal.Mobility</t>
   </si>
   <si>
     <t>Mobility device provided</t>
@@ -6606,7 +6606,7 @@
     <t>&amp;Mobility device provided</t>
   </si>
   <si>
-    <t>risk.healthGoalPain</t>
+    <t>risk.health.goal.Pain</t>
   </si>
   <si>
     <t>Pain managed</t>
@@ -6615,7 +6615,7 @@
     <t>&amp;Pain managed</t>
   </si>
   <si>
-    <t>risk.socialRequirementContact</t>
+    <t>risk.social.requirement.Contact</t>
   </si>
   <si>
     <t>Contact with community</t>
@@ -6624,7 +6624,7 @@
     <t>&amp;Contact with community</t>
   </si>
   <si>
-    <t>risk.socialRequirementInclusion</t>
+    <t>risk.social.requirement.Inclusion</t>
   </si>
   <si>
     <t>Inclusion in family</t>
@@ -6633,7 +6633,7 @@
     <t>&amp;Inclusion in family</t>
   </si>
   <si>
-    <t>risk.socialRequirementTraining</t>
+    <t>risk.social.requirement.Training</t>
   </si>
   <si>
     <t>Training for family members</t>
@@ -6642,7 +6642,7 @@
     <t>&amp;Training for family members</t>
   </si>
   <si>
-    <t>risk.socialGoalCommunity</t>
+    <t>risk.social.goal.Community</t>
   </si>
   <si>
     <t>Take part in a community event</t>
@@ -6651,7 +6651,7 @@
     <t>&amp;Take part in a community event</t>
   </si>
   <si>
-    <t>risk.socialGoalInclusion</t>
+    <t>risk.social.goal.Inclusion</t>
   </si>
   <si>
     <t>Inclusion in family time</t>
@@ -6660,7 +6660,7 @@
     <t>&amp;Inclusion in family time</t>
   </si>
   <si>
-    <t>risk.nutritionRequirementDiabetic</t>
+    <t>risk.nutrition.requirement.Diabetic</t>
   </si>
   <si>
     <t>Special dietary need - diabetic</t>
@@ -6669,7 +6669,7 @@
     <t>&amp;Special dietary need - diabetic</t>
   </si>
   <si>
-    <t>risk.nutritionRequirementAllergies</t>
+    <t>risk.nutrition.requirement.Allergies</t>
   </si>
   <si>
     <t>Special dietary need - allergies</t>
@@ -6678,7 +6678,7 @@
     <t>&amp;Special dietary need - allergies</t>
   </si>
   <si>
-    <t>risk.nutritionRequirementMalnutrition</t>
+    <t>risk.nutrition.requirement.Malnutrition</t>
   </si>
   <si>
     <t>Special dietary need - malnutrition</t>
@@ -6687,7 +6687,7 @@
     <t>&amp;Special dietary need - malnutrition</t>
   </si>
   <si>
-    <t>risk.nutritionRequirementTraining</t>
+    <t>risk.nutrition.requirement.Training</t>
   </si>
   <si>
     <t>Nutrition training</t>
@@ -6696,7 +6696,7 @@
     <t>&amp;Nutrition training</t>
   </si>
   <si>
-    <t>risk.nutritionRequirementAgricultural</t>
+    <t>risk.nutrition.requirement.Agricultural</t>
   </si>
   <si>
     <t>Inclusion in Agricultural project</t>
@@ -6705,7 +6705,7 @@
     <t>&amp;Inclusion in Agricultural project</t>
   </si>
   <si>
-    <t>risk.nutritionGoalManageDiet</t>
+    <t>risk.nutrition.goal.ManageDiet</t>
   </si>
   <si>
     <t>Manage diet to meet needs</t>
@@ -6714,7 +6714,7 @@
     <t>&amp;Manage diet to meet needs</t>
   </si>
   <si>
-    <t>risk.nutritionGoalSustainable</t>
+    <t>risk.nutrition.goal.Sustainable</t>
   </si>
   <si>
     <t>Sustainable food source</t>
@@ -6723,7 +6723,7 @@
     <t>&amp;Sustainable food source</t>
   </si>
   <si>
-    <t>risk.educationRequirementSchool</t>
+    <t>risk.education.requirement.School</t>
   </si>
   <si>
     <t>Attend school</t>
@@ -6732,7 +6732,7 @@
     <t>&amp;Attend school</t>
   </si>
   <si>
-    <t>risk.educationRequirementVocational</t>
+    <t>risk.education.requirement.Vocational</t>
   </si>
   <si>
     <t>Vocational training</t>
@@ -6741,7 +6741,7 @@
     <t>&amp;Vocational training</t>
   </si>
   <si>
-    <t>risk.educationRequirementFamily</t>
+    <t>risk.education.requirement.Family</t>
   </si>
   <si>
     <t>Training for family - learning through play</t>
@@ -6750,7 +6750,7 @@
     <t>&amp;Training for family - learning through play</t>
   </si>
   <si>
-    <t>risk.educationGoalEducation</t>
+    <t>risk.education.goal.Education</t>
   </si>
   <si>
     <t>Have an education</t>
@@ -6759,7 +6759,7 @@
     <t>&amp;Have an education</t>
   </si>
   <si>
-    <t>risk.educationGoalIncome</t>
+    <t>risk.education.goal.Income</t>
   </si>
   <si>
     <t>Sustainable source of income</t>
@@ -6768,7 +6768,7 @@
     <t>&amp;Sustainable source of income</t>
   </si>
   <si>
-    <t>risk.educationGoalChild</t>
+    <t>risk.education.goal.Child</t>
   </si>
   <si>
     <t>Child ready to start school</t>
@@ -6777,7 +6777,7 @@
     <t>&amp;Child ready to start school</t>
   </si>
   <si>
-    <t>risk.mentalRequirementMedical</t>
+    <t>risk.mental.requirement.Medical</t>
   </si>
   <si>
     <t>Needs medical attention</t>
@@ -6786,7 +6786,7 @@
     <t>&amp;Needs medical attention</t>
   </si>
   <si>
-    <t>risk.mentalRequirementFamily</t>
+    <t>risk.mental.requirement.Family</t>
   </si>
   <si>
     <t>Promote understanding in the family</t>
@@ -6795,7 +6795,7 @@
     <t>&amp;Promote understanding in the family</t>
   </si>
   <si>
-    <t>risk.mentalRequirementCommunity</t>
+    <t>risk.mental.requirement.Community</t>
   </si>
   <si>
     <t>Promote understanding in the community</t>
@@ -6804,7 +6804,7 @@
     <t>&amp;Promote understanding in the community</t>
   </si>
   <si>
-    <t>risk.mentalRequirementRefer</t>
+    <t>risk.mental.requirement.Refer</t>
   </si>
   <si>
     <t>Refer to mental health agencies</t>
@@ -6813,7 +6813,7 @@
     <t>&amp;Refer to mental health agencies</t>
   </si>
   <si>
-    <t>risk.mentalRequirementCounsellingStressTrauma</t>
+    <t>risk.mental.requirement.CounsellingStressTrauma</t>
   </si>
   <si>
     <t>Advice and counselling - stress and trauma</t>
@@ -6822,7 +6822,7 @@
     <t>&amp;Advice and counselling - stress and trauma</t>
   </si>
   <si>
-    <t>risk.mentalRequirementCounsellingOther</t>
+    <t>risk.mental.requirement.CounsellingOther</t>
   </si>
   <si>
     <t>Advice and counselling - other</t>
@@ -6831,10 +6831,10 @@
     <t>&amp;Advice and counselling - other</t>
   </si>
   <si>
-    <t>risk.mentalGoalFamily</t>
-  </si>
-  <si>
-    <t>risk.mentalGoalCommunity</t>
+    <t>risk.mental.goal.Family</t>
+  </si>
+  <si>
+    <t>risk.mental.goal.Community</t>
   </si>
   <si>
     <t>Inclusion in community</t>
@@ -6843,7 +6843,7 @@
     <t>&amp;Inclusion in community</t>
   </si>
   <si>
-    <t>risk.mentalGoalMedical</t>
+    <t>risk.mental.goal.Medical</t>
   </si>
   <si>
     <t>Medical assistance provided</t>
@@ -6852,7 +6852,7 @@
     <t>&amp;Medical assistance provided</t>
   </si>
   <si>
-    <t>risk.mentalGoalAgency</t>
+    <t>risk.mental.goal.Agency</t>
   </si>
   <si>
     <t>Seen by mental health agency</t>
@@ -6861,7 +6861,7 @@
     <t>&amp;Seen by mental health agency</t>
   </si>
   <si>
-    <t>risk.mentalGoalImprovement</t>
+    <t>risk.mental.goal.Improvement</t>
   </si>
   <si>
     <t>Improvement in mental health</t>
@@ -6870,7 +6870,7 @@
     <t>&amp;Improvement in mental health</t>
   </si>
   <si>
-    <t>risk.mentalGoalReduction</t>
+    <t>risk.mental.goal.Reduction</t>
   </si>
   <si>
     <t>Reduction of stress and trauma</t>
@@ -6879,7 +6879,7 @@
     <t>&amp;Reduction of stress and trauma</t>
   </si>
   <si>
-    <t>risk.mentalGoalImprovements</t>
+    <t>risk.mental.goal.Improvements</t>
   </si>
   <si>
     <t>&amp;Improvements</t>

</xml_diff>

<commit_message>
feat: add dropdowns to mobile and refactor to use keys, add image subtitle to new client form
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="2286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="2289">
   <si>
     <t>Key</t>
   </si>
@@ -6883,6 +6883,15 @@
   </si>
   <si>
     <t>&amp;Improvements</t>
+  </si>
+  <si>
+    <t>clientFields.imageSubtitle</t>
+  </si>
+  <si>
+    <t>Press the icon to upload an image.</t>
+  </si>
+  <si>
+    <t>&amp;Press the icon to upload an image.</t>
   </si>
 </sst>
 </file>
@@ -17663,7 +17672,17 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1">
+      <c r="A816" s="40" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B816" s="16" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C816" s="16" t="s">
+        <v>2288</v>
+      </c>
+    </row>
     <row r="817" ht="15.75" customHeight="1"/>
     <row r="818" ht="15.75" customHeight="1"/>
     <row r="819" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
update cancellation reason "other" placeholder text and adjust mobile dropdown styling
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="2289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="2292">
   <si>
     <t>Key</t>
   </si>
@@ -6892,6 +6892,15 @@
   </si>
   <si>
     <t>&amp;Press the icon to upload an image.</t>
+  </si>
+  <si>
+    <t>risks.specify</t>
+  </si>
+  <si>
+    <t>Please specify</t>
+  </si>
+  <si>
+    <t>&amp;Please specify</t>
   </si>
 </sst>
 </file>
@@ -17683,7 +17692,17 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1">
+      <c r="A817" s="40" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B817" s="16" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C817" s="16" t="s">
+        <v>2291</v>
+      </c>
+    </row>
     <row r="818" ht="15.75" customHeight="1"/>
     <row r="819" ht="15.75" customHeight="1"/>
     <row r="820" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
update to support other in new client for backend and handle issue of other field if they type in something that matches a translation key
</commit_message>
<xml_diff>
--- a/common/src/locales/Translations_CBR_main.xlsx
+++ b/common/src/locales/Translations_CBR_main.xlsx
@@ -6492,7 +6492,7 @@
     <t>&amp;You may have unsaved changes. Are you sure you want to go back?</t>
   </si>
   <si>
-    <t>cancellation.dead</t>
+    <t>cancellation._$dead</t>
   </si>
   <si>
     <t>Patient has died</t>
@@ -6501,7 +6501,7 @@
     <t>&amp;Patient has died</t>
   </si>
   <si>
-    <t>cancellation.moved</t>
+    <t>cancellation._$moved</t>
   </si>
   <si>
     <t>Patient has moved away</t>
@@ -6510,7 +6510,7 @@
     <t>&amp;Patient has moved away</t>
   </si>
   <si>
-    <t>cancellation.circumstances</t>
+    <t>cancellation._$circumstances</t>
   </si>
   <si>
     <t>Patient's circumstances have changed</t>
@@ -6519,7 +6519,7 @@
     <t>&amp;Patient's circumstances have changed</t>
   </si>
   <si>
-    <t>cancellation.abandoned</t>
+    <t>cancellation._$abandoned</t>
   </si>
   <si>
     <t>Patient has abandoned this goal</t>
@@ -6528,7 +6528,7 @@
     <t>&amp;Patient has abandoned this goal</t>
   </si>
   <si>
-    <t>cancellation.unwilling</t>
+    <t>cancellation._$unwilling</t>
   </si>
   <si>
     <t>Patient is no longer willing to work with us</t>
@@ -6537,7 +6537,7 @@
     <t>&amp;Patient is no longer willing to work with us</t>
   </si>
   <si>
-    <t>risk.health.requirement.Malaria</t>
+    <t>risk.health.requirement._$Malaria</t>
   </si>
   <si>
     <t>Malaria treatment</t>
@@ -6546,7 +6546,7 @@
     <t>&amp;Malaria treatment</t>
   </si>
   <si>
-    <t>risk.health.requirement.Medical</t>
+    <t>risk.health.requirement._$Medical</t>
   </si>
   <si>
     <t>Medical assistance</t>
@@ -6555,7 +6555,7 @@
     <t>&amp;Medical assistance</t>
   </si>
   <si>
-    <t>risk.health.requirement.Wound</t>
+    <t>risk.health.requirement._$Wound</t>
   </si>
   <si>
     <t>Wound care for pressure sores</t>
@@ -6564,7 +6564,7 @@
     <t>&amp;Wound care for pressure sores</t>
   </si>
   <si>
-    <t>risk.health.requirement.Mobility</t>
+    <t>risk.health.requirement._$Mobility</t>
   </si>
   <si>
     <t>Mobility device - crutches</t>
@@ -6573,13 +6573,13 @@
     <t>&amp;Mobility device - crutches</t>
   </si>
   <si>
-    <t>risk.health.requirement.Physiotherapy</t>
+    <t>risk.health.requirement._$Physiotherapy</t>
   </si>
   <si>
     <t>&amp;Physiotherapy</t>
   </si>
   <si>
-    <t>risk.health.goal.Medical</t>
+    <t>risk.health.goal._$Medical</t>
   </si>
   <si>
     <t>Medical treatment provided</t>
@@ -6588,7 +6588,7 @@
     <t>&amp;Medical treatment provided</t>
   </si>
   <si>
-    <t>risk.health.goal.Sores</t>
+    <t>risk.health.goal._$Sores</t>
   </si>
   <si>
     <t>Sores managed/healed</t>
@@ -6597,7 +6597,7 @@
     <t>&amp;Sores managed/healed</t>
   </si>
   <si>
-    <t>risk.health.goal.Mobility</t>
+    <t>risk.health.goal._$Mobility</t>
   </si>
   <si>
     <t>Mobility device provided</t>
@@ -6606,7 +6606,7 @@
     <t>&amp;Mobility device provided</t>
   </si>
   <si>
-    <t>risk.health.goal.Pain</t>
+    <t>risk.health.goal._$Pain</t>
   </si>
   <si>
     <t>Pain managed</t>
@@ -6615,7 +6615,7 @@
     <t>&amp;Pain managed</t>
   </si>
   <si>
-    <t>risk.social.requirement.Contact</t>
+    <t>risk.social.requirement._$Contact</t>
   </si>
   <si>
     <t>Contact with community</t>
@@ -6624,7 +6624,7 @@
     <t>&amp;Contact with community</t>
   </si>
   <si>
-    <t>risk.social.requirement.Inclusion</t>
+    <t>risk.social.requirement._$Inclusion</t>
   </si>
   <si>
     <t>Inclusion in family</t>
@@ -6633,7 +6633,7 @@
     <t>&amp;Inclusion in family</t>
   </si>
   <si>
-    <t>risk.social.requirement.Training</t>
+    <t>risk.social.requirement._$Training</t>
   </si>
   <si>
     <t>Training for family members</t>
@@ -6642,7 +6642,7 @@
     <t>&amp;Training for family members</t>
   </si>
   <si>
-    <t>risk.social.goal.Community</t>
+    <t>risk.social.goal._$Community</t>
   </si>
   <si>
     <t>Take part in a community event</t>
@@ -6651,7 +6651,7 @@
     <t>&amp;Take part in a community event</t>
   </si>
   <si>
-    <t>risk.social.goal.Inclusion</t>
+    <t>risk.social.goal._$Inclusion</t>
   </si>
   <si>
     <t>Inclusion in family time</t>
@@ -6660,7 +6660,7 @@
     <t>&amp;Inclusion in family time</t>
   </si>
   <si>
-    <t>risk.nutrition.requirement.Diabetic</t>
+    <t>risk.nutrition.requirement._$Diabetic</t>
   </si>
   <si>
     <t>Special dietary need - diabetic</t>
@@ -6669,7 +6669,7 @@
     <t>&amp;Special dietary need - diabetic</t>
   </si>
   <si>
-    <t>risk.nutrition.requirement.Allergies</t>
+    <t>risk.nutrition.requirement._$Allergies</t>
   </si>
   <si>
     <t>Special dietary need - allergies</t>
@@ -6678,7 +6678,7 @@
     <t>&amp;Special dietary need - allergies</t>
   </si>
   <si>
-    <t>risk.nutrition.requirement.Malnutrition</t>
+    <t>risk.nutrition.requirement._$Malnutrition</t>
   </si>
   <si>
     <t>Special dietary need - malnutrition</t>
@@ -6687,7 +6687,7 @@
     <t>&amp;Special dietary need - malnutrition</t>
   </si>
   <si>
-    <t>risk.nutrition.requirement.Training</t>
+    <t>risk.nutrition.requirement._$Training</t>
   </si>
   <si>
     <t>Nutrition training</t>
@@ -6696,7 +6696,7 @@
     <t>&amp;Nutrition training</t>
   </si>
   <si>
-    <t>risk.nutrition.requirement.Agricultural</t>
+    <t>risk.nutrition.requirement._$Agricultural</t>
   </si>
   <si>
     <t>Inclusion in Agricultural project</t>
@@ -6705,7 +6705,7 @@
     <t>&amp;Inclusion in Agricultural project</t>
   </si>
   <si>
-    <t>risk.nutrition.goal.ManageDiet</t>
+    <t>risk.nutrition.goal._$ManageDiet</t>
   </si>
   <si>
     <t>Manage diet to meet needs</t>
@@ -6714,7 +6714,7 @@
     <t>&amp;Manage diet to meet needs</t>
   </si>
   <si>
-    <t>risk.nutrition.goal.Sustainable</t>
+    <t>risk.nutrition.goal._$Sustainable</t>
   </si>
   <si>
     <t>Sustainable food source</t>
@@ -6723,7 +6723,7 @@
     <t>&amp;Sustainable food source</t>
   </si>
   <si>
-    <t>risk.education.requirement.School</t>
+    <t>risk.education.requirement._$School</t>
   </si>
   <si>
     <t>Attend school</t>
@@ -6732,7 +6732,7 @@
     <t>&amp;Attend school</t>
   </si>
   <si>
-    <t>risk.education.requirement.Vocational</t>
+    <t>risk.education.requirement._$Vocational</t>
   </si>
   <si>
     <t>Vocational training</t>
@@ -6741,7 +6741,7 @@
     <t>&amp;Vocational training</t>
   </si>
   <si>
-    <t>risk.education.requirement.Family</t>
+    <t>risk.education.requirement._$Family</t>
   </si>
   <si>
     <t>Training for family - learning through play</t>
@@ -6750,7 +6750,7 @@
     <t>&amp;Training for family - learning through play</t>
   </si>
   <si>
-    <t>risk.education.goal.Education</t>
+    <t>risk.education.goal._$Education</t>
   </si>
   <si>
     <t>Have an education</t>
@@ -6759,7 +6759,7 @@
     <t>&amp;Have an education</t>
   </si>
   <si>
-    <t>risk.education.goal.Income</t>
+    <t>risk.education.goal._$Income</t>
   </si>
   <si>
     <t>Sustainable source of income</t>
@@ -6768,7 +6768,7 @@
     <t>&amp;Sustainable source of income</t>
   </si>
   <si>
-    <t>risk.education.goal.Child</t>
+    <t>risk.education.goal._$Child</t>
   </si>
   <si>
     <t>Child ready to start school</t>
@@ -6777,7 +6777,7 @@
     <t>&amp;Child ready to start school</t>
   </si>
   <si>
-    <t>risk.mental.requirement.Medical</t>
+    <t>risk.mental.requirement._$Medical</t>
   </si>
   <si>
     <t>Needs medical attention</t>
@@ -6786,7 +6786,7 @@
     <t>&amp;Needs medical attention</t>
   </si>
   <si>
-    <t>risk.mental.requirement.Family</t>
+    <t>risk.mental.requirement._$Family</t>
   </si>
   <si>
     <t>Promote understanding in the family</t>
@@ -6795,7 +6795,7 @@
     <t>&amp;Promote understanding in the family</t>
   </si>
   <si>
-    <t>risk.mental.requirement.Community</t>
+    <t>risk.mental.requirement._$Community</t>
   </si>
   <si>
     <t>Promote understanding in the community</t>
@@ -6804,7 +6804,7 @@
     <t>&amp;Promote understanding in the community</t>
   </si>
   <si>
-    <t>risk.mental.requirement.Refer</t>
+    <t>risk.mental.requirement._$Refer</t>
   </si>
   <si>
     <t>Refer to mental health agencies</t>
@@ -6813,7 +6813,7 @@
     <t>&amp;Refer to mental health agencies</t>
   </si>
   <si>
-    <t>risk.mental.requirement.CounsellingStressTrauma</t>
+    <t>risk.mental.requirement._$CounsellingStressTrauma</t>
   </si>
   <si>
     <t>Advice and counselling - stress and trauma</t>
@@ -6822,7 +6822,7 @@
     <t>&amp;Advice and counselling - stress and trauma</t>
   </si>
   <si>
-    <t>risk.mental.requirement.CounsellingOther</t>
+    <t>risk.mental.requirement._$CounsellingOther</t>
   </si>
   <si>
     <t>Advice and counselling - other</t>
@@ -6831,10 +6831,10 @@
     <t>&amp;Advice and counselling - other</t>
   </si>
   <si>
-    <t>risk.mental.goal.Family</t>
-  </si>
-  <si>
-    <t>risk.mental.goal.Community</t>
+    <t>risk.mental.goal._$Family</t>
+  </si>
+  <si>
+    <t>risk.mental.goal._$Community</t>
   </si>
   <si>
     <t>Inclusion in community</t>
@@ -6843,7 +6843,7 @@
     <t>&amp;Inclusion in community</t>
   </si>
   <si>
-    <t>risk.mental.goal.Medical</t>
+    <t>risk.mental.goal._$Medical</t>
   </si>
   <si>
     <t>Medical assistance provided</t>
@@ -6852,7 +6852,7 @@
     <t>&amp;Medical assistance provided</t>
   </si>
   <si>
-    <t>risk.mental.goal.Agency</t>
+    <t>risk.mental.goal._$Agency</t>
   </si>
   <si>
     <t>Seen by mental health agency</t>
@@ -6861,7 +6861,7 @@
     <t>&amp;Seen by mental health agency</t>
   </si>
   <si>
-    <t>risk.mental.goal.Improvement</t>
+    <t>risk.mental.goal._$Improvement</t>
   </si>
   <si>
     <t>Improvement in mental health</t>
@@ -6870,7 +6870,7 @@
     <t>&amp;Improvement in mental health</t>
   </si>
   <si>
-    <t>risk.mental.goal.Reduction</t>
+    <t>risk.mental.goal._$Reduction</t>
   </si>
   <si>
     <t>Reduction of stress and trauma</t>
@@ -6879,7 +6879,7 @@
     <t>&amp;Reduction of stress and trauma</t>
   </si>
   <si>
-    <t>risk.mental.goal.Improvements</t>
+    <t>risk.mental.goal._$Improvements</t>
   </si>
   <si>
     <t>&amp;Improvements</t>

</xml_diff>